<commit_message>
Added mu name to the spreadsheet.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,7 +14,7 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -709,9 +709,6 @@
     <t>test run</t>
   </si>
   <si>
-    <t>adelikat</t>
-  </si>
-  <si>
     <t>4th screen</t>
   </si>
   <si>
@@ -737,6 +734,9 @@
   </si>
   <si>
     <t>Text screen done</t>
+  </si>
+  <si>
+    <t>adelikat &amp; sonikkustar</t>
   </si>
 </sst>
 </file>
@@ -1954,6 +1954,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1975,29 +1978,29 @@
     <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2033,20 +2036,34 @@
     <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2055,23 +2072,6 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2384,7 +2384,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2400,16 +2400,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="155" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="154"/>
+      <c r="C1" s="156" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="157"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65535)</f>
@@ -2455,7 +2455,7 @@
         <v>159</v>
       </c>
       <c r="B3" s="142" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C3" s="143"/>
       <c r="D3" s="143"/>
@@ -2487,10 +2487,10 @@
       <c r="B5" s="147" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2506,10 +2506,10 @@
       <c r="B6" s="147" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="153" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="153"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2527,7 +2527,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="158" t="s">
         <v>187</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="150"/>
+      <c r="A9" s="151"/>
       <c r="B9" s="98" t="s">
         <v>183</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="150"/>
+      <c r="A10" s="151"/>
       <c r="B10" s="148" t="s">
         <v>212</v>
       </c>
@@ -2579,9 +2579,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="150"/>
+      <c r="A11" s="151"/>
       <c r="B11" s="148" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C11" s="101"/>
       <c r="D11" s="101">
@@ -2593,13 +2593,13 @@
       </c>
       <c r="F11" s="105"/>
       <c r="H11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" outlineLevel="1">
+      <c r="A12" s="151"/>
+      <c r="B12" s="148" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="150"/>
-      <c r="B12" s="148" t="s">
-        <v>219</v>
       </c>
       <c r="C12" s="101"/>
       <c r="D12" s="101">
@@ -2612,9 +2612,9 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="150"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="148" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C13" s="101"/>
       <c r="D13" s="101">
@@ -2627,9 +2627,9 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="150"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="148" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" s="101"/>
       <c r="D14" s="101">
@@ -2642,9 +2642,9 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="150"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="101"/>
       <c r="D15" s="101">
@@ -2657,7 +2657,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A16" s="150"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="98" t="s">
         <v>186</v>
       </c>
@@ -2700,8 +2700,8 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="151" t="s">
-        <v>223</v>
+      <c r="A19" s="152" t="s">
+        <v>222</v>
       </c>
       <c r="B19" s="109" t="s">
         <v>181</v>
@@ -2720,7 +2720,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="150"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="98" t="s">
         <v>183</v>
       </c>
@@ -2735,9 +2735,9 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A21" s="150"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="101"/>
       <c r="D21" s="101">
@@ -2750,9 +2750,9 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A22" s="150"/>
-      <c r="B22" s="213" t="s">
-        <v>224</v>
+      <c r="A22" s="151"/>
+      <c r="B22" s="149" t="s">
+        <v>223</v>
       </c>
       <c r="C22" s="101"/>
       <c r="D22" s="101">
@@ -2765,9 +2765,9 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A23" s="150"/>
-      <c r="B23" s="213" t="s">
-        <v>225</v>
+      <c r="A23" s="151"/>
+      <c r="B23" s="149" t="s">
+        <v>224</v>
       </c>
       <c r="C23" s="101"/>
       <c r="D23" s="101">
@@ -2780,7 +2780,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A24" s="150"/>
+      <c r="A24" s="151"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2791,7 +2791,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A25" s="150"/>
+      <c r="A25" s="151"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2802,7 +2802,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A26" s="150"/>
+      <c r="A26" s="151"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2813,7 +2813,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A27" s="150"/>
+      <c r="A27" s="151"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2824,7 +2824,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A28" s="150"/>
+      <c r="A28" s="151"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2835,7 +2835,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A29" s="150"/>
+      <c r="A29" s="151"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2846,7 +2846,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A30" s="150"/>
+      <c r="A30" s="151"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2857,7 +2857,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A31" s="150"/>
+      <c r="A31" s="151"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2868,7 +2868,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A32" s="150"/>
+      <c r="A32" s="151"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2879,7 +2879,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A33" s="150"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="98" t="s">
         <v>186</v>
       </c>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="149" t="s">
+      <c r="A36" s="150" t="s">
         <v>169</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2938,7 +2938,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A37" s="150"/>
+      <c r="A37" s="151"/>
       <c r="B37" s="98" t="s">
         <v>183</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A38" s="150"/>
+      <c r="A38" s="151"/>
       <c r="B38" s="100"/>
       <c r="C38" s="101"/>
       <c r="D38" s="101"/>
@@ -2962,7 +2962,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A39" s="150"/>
+      <c r="A39" s="151"/>
       <c r="B39" s="100"/>
       <c r="C39" s="101"/>
       <c r="D39" s="101"/>
@@ -2973,7 +2973,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A40" s="150"/>
+      <c r="A40" s="151"/>
       <c r="B40" s="100"/>
       <c r="C40" s="101"/>
       <c r="D40" s="101"/>
@@ -2984,7 +2984,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A41" s="150"/>
+      <c r="A41" s="151"/>
       <c r="B41" s="100"/>
       <c r="C41" s="101"/>
       <c r="D41" s="101"/>
@@ -2995,7 +2995,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A42" s="150"/>
+      <c r="A42" s="151"/>
       <c r="B42" s="100"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -3006,7 +3006,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A43" s="150"/>
+      <c r="A43" s="151"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3017,7 +3017,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A44" s="150"/>
+      <c r="A44" s="151"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3028,7 +3028,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A45" s="150"/>
+      <c r="A45" s="151"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3039,7 +3039,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A46" s="150"/>
+      <c r="A46" s="151"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3050,7 +3050,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A47" s="150"/>
+      <c r="A47" s="151"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3061,7 +3061,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A48" s="150"/>
+      <c r="A48" s="151"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3072,7 +3072,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A49" s="150"/>
+      <c r="A49" s="151"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3083,7 +3083,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A50" s="150"/>
+      <c r="A50" s="151"/>
       <c r="B50" s="98" t="s">
         <v>186</v>
       </c>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="151" t="s">
+      <c r="A53" s="152" t="s">
         <v>170</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3142,7 +3142,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A54" s="150"/>
+      <c r="A54" s="151"/>
       <c r="B54" s="98" t="s">
         <v>183</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="F54" s="104"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A55" s="150"/>
+      <c r="A55" s="151"/>
       <c r="B55" s="100"/>
       <c r="C55" s="101"/>
       <c r="D55" s="101"/>
@@ -3166,7 +3166,7 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A56" s="150"/>
+      <c r="A56" s="151"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3177,7 +3177,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A57" s="150"/>
+      <c r="A57" s="151"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3188,7 +3188,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A58" s="150"/>
+      <c r="A58" s="151"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3199,7 +3199,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A59" s="150"/>
+      <c r="A59" s="151"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3210,7 +3210,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A60" s="150"/>
+      <c r="A60" s="151"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3221,7 +3221,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A61" s="150"/>
+      <c r="A61" s="151"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3232,7 +3232,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A62" s="150"/>
+      <c r="A62" s="151"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3243,7 +3243,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A63" s="150"/>
+      <c r="A63" s="151"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3254,7 +3254,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A64" s="150"/>
+      <c r="A64" s="151"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3265,7 +3265,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A65" s="150"/>
+      <c r="A65" s="151"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3276,7 +3276,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A66" s="150"/>
+      <c r="A66" s="151"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3287,7 +3287,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A67" s="150"/>
+      <c r="A67" s="151"/>
       <c r="B67" s="98" t="s">
         <v>186</v>
       </c>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="149" t="s">
+      <c r="A70" s="150" t="s">
         <v>171</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3346,7 +3346,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A71" s="150"/>
+      <c r="A71" s="151"/>
       <c r="B71" s="98" t="s">
         <v>183</v>
       </c>
@@ -3359,7 +3359,7 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A72" s="150"/>
+      <c r="A72" s="151"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3370,7 +3370,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A73" s="150"/>
+      <c r="A73" s="151"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3381,7 +3381,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A74" s="150"/>
+      <c r="A74" s="151"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3392,7 +3392,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A75" s="150"/>
+      <c r="A75" s="151"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3403,7 +3403,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A76" s="150"/>
+      <c r="A76" s="151"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3414,7 +3414,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A77" s="150"/>
+      <c r="A77" s="151"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3425,7 +3425,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A78" s="150"/>
+      <c r="A78" s="151"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3436,7 +3436,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A79" s="150"/>
+      <c r="A79" s="151"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3447,7 +3447,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A80" s="150"/>
+      <c r="A80" s="151"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3458,7 +3458,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A81" s="150"/>
+      <c r="A81" s="151"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3469,7 +3469,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A82" s="150"/>
+      <c r="A82" s="151"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3480,7 +3480,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A83" s="150"/>
+      <c r="A83" s="151"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3491,7 +3491,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A84" s="150"/>
+      <c r="A84" s="151"/>
       <c r="B84" s="98" t="s">
         <v>186</v>
       </c>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="151" t="s">
+      <c r="A87" s="152" t="s">
         <v>172</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3550,7 +3550,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A88" s="150"/>
+      <c r="A88" s="151"/>
       <c r="B88" s="98" t="s">
         <v>183</v>
       </c>
@@ -3563,7 +3563,7 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A89" s="150"/>
+      <c r="A89" s="151"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3574,7 +3574,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A90" s="150"/>
+      <c r="A90" s="151"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3585,7 +3585,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A91" s="150"/>
+      <c r="A91" s="151"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3596,7 +3596,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A92" s="150"/>
+      <c r="A92" s="151"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3607,7 +3607,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A93" s="150"/>
+      <c r="A93" s="151"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3618,7 +3618,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A94" s="150"/>
+      <c r="A94" s="151"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3629,7 +3629,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A95" s="150"/>
+      <c r="A95" s="151"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3640,7 +3640,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A96" s="150"/>
+      <c r="A96" s="151"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3651,7 +3651,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A97" s="150"/>
+      <c r="A97" s="151"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3662,7 +3662,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A98" s="150"/>
+      <c r="A98" s="151"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3673,7 +3673,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A99" s="150"/>
+      <c r="A99" s="151"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3684,7 +3684,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A100" s="150"/>
+      <c r="A100" s="151"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3695,7 +3695,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A101" s="150"/>
+      <c r="A101" s="151"/>
       <c r="B101" s="98" t="s">
         <v>186</v>
       </c>
@@ -3733,7 +3733,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="149" t="s">
+      <c r="A104" s="150" t="s">
         <v>173</v>
       </c>
       <c r="B104" s="113" t="s">
@@ -3753,7 +3753,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A105" s="150"/>
+      <c r="A105" s="151"/>
       <c r="B105" s="98" t="s">
         <v>183</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="F105" s="104"/>
     </row>
     <row r="106" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A106" s="150"/>
+      <c r="A106" s="151"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3777,7 +3777,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A107" s="150"/>
+      <c r="A107" s="151"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3788,7 +3788,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A108" s="150"/>
+      <c r="A108" s="151"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3799,7 +3799,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A109" s="150"/>
+      <c r="A109" s="151"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3810,7 +3810,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A110" s="150"/>
+      <c r="A110" s="151"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3821,7 +3821,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A111" s="150"/>
+      <c r="A111" s="151"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3832,7 +3832,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A112" s="150"/>
+      <c r="A112" s="151"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3843,7 +3843,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A113" s="150"/>
+      <c r="A113" s="151"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3854,7 +3854,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A114" s="150"/>
+      <c r="A114" s="151"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3865,7 +3865,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A115" s="150"/>
+      <c r="A115" s="151"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3876,7 +3876,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A116" s="150"/>
+      <c r="A116" s="151"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3887,7 +3887,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A117" s="150"/>
+      <c r="A117" s="151"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -3898,7 +3898,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A118" s="150"/>
+      <c r="A118" s="151"/>
       <c r="B118" s="98" t="s">
         <v>186</v>
       </c>
@@ -3936,7 +3936,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="151" t="s">
+      <c r="A121" s="152" t="s">
         <v>174</v>
       </c>
       <c r="B121" s="109" t="s">
@@ -3956,7 +3956,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A122" s="150"/>
+      <c r="A122" s="151"/>
       <c r="B122" s="98" t="s">
         <v>183</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="F122" s="104"/>
     </row>
     <row r="123" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A123" s="150"/>
+      <c r="A123" s="151"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -3980,7 +3980,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A124" s="150"/>
+      <c r="A124" s="151"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -3991,7 +3991,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A125" s="150"/>
+      <c r="A125" s="151"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4002,7 +4002,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A126" s="150"/>
+      <c r="A126" s="151"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4013,7 +4013,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A127" s="150"/>
+      <c r="A127" s="151"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4024,7 +4024,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A128" s="150"/>
+      <c r="A128" s="151"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4035,7 +4035,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A129" s="150"/>
+      <c r="A129" s="151"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4046,7 +4046,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A130" s="150"/>
+      <c r="A130" s="151"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4057,7 +4057,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A131" s="150"/>
+      <c r="A131" s="151"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4068,7 +4068,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A132" s="150"/>
+      <c r="A132" s="151"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4079,7 +4079,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A133" s="150"/>
+      <c r="A133" s="151"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4090,7 +4090,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A134" s="150"/>
+      <c r="A134" s="151"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4101,7 +4101,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A135" s="150"/>
+      <c r="A135" s="151"/>
       <c r="B135" s="98" t="s">
         <v>186</v>
       </c>
@@ -4139,7 +4139,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="149" t="s">
+      <c r="A138" s="150" t="s">
         <v>175</v>
       </c>
       <c r="B138" s="113" t="s">
@@ -4159,7 +4159,7 @@
       </c>
     </row>
     <row r="139" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A139" s="150"/>
+      <c r="A139" s="151"/>
       <c r="B139" s="98" t="s">
         <v>183</v>
       </c>
@@ -4172,7 +4172,7 @@
       <c r="F139" s="104"/>
     </row>
     <row r="140" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A140" s="150"/>
+      <c r="A140" s="151"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4183,7 +4183,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A141" s="150"/>
+      <c r="A141" s="151"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4194,7 +4194,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A142" s="150"/>
+      <c r="A142" s="151"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4205,7 +4205,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A143" s="150"/>
+      <c r="A143" s="151"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4216,7 +4216,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A144" s="150"/>
+      <c r="A144" s="151"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4227,7 +4227,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A145" s="150"/>
+      <c r="A145" s="151"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4238,7 +4238,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="150"/>
+      <c r="A146" s="151"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4249,7 +4249,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="150"/>
+      <c r="A147" s="151"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4260,7 +4260,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="150"/>
+      <c r="A148" s="151"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4271,7 +4271,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="150"/>
+      <c r="A149" s="151"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4282,7 +4282,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="150"/>
+      <c r="A150" s="151"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4293,7 +4293,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="150"/>
+      <c r="A151" s="151"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4304,7 +4304,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A152" s="150"/>
+      <c r="A152" s="151"/>
       <c r="B152" s="98" t="s">
         <v>186</v>
       </c>
@@ -4343,6 +4343,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A138:A152"/>
+    <mergeCell ref="A104:A118"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4351,11 +4356,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4387,13 +4387,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4423,18 +4423,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4586,9 +4586,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="161"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="165"/>
+      <c r="E21" s="165"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4739,9 +4739,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="158"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -4892,9 +4892,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="158"/>
-      <c r="D55" s="159"/>
-      <c r="E55" s="159"/>
+      <c r="C55" s="162"/>
+      <c r="D55" s="163"/>
+      <c r="E55" s="163"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5045,9 +5045,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="158"/>
-      <c r="D72" s="159"/>
-      <c r="E72" s="159"/>
+      <c r="C72" s="162"/>
+      <c r="D72" s="163"/>
+      <c r="E72" s="163"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5198,9 +5198,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="158"/>
-      <c r="D89" s="159"/>
-      <c r="E89" s="159"/>
+      <c r="C89" s="162"/>
+      <c r="D89" s="163"/>
+      <c r="E89" s="163"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5351,9 +5351,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="158"/>
-      <c r="D106" s="159"/>
-      <c r="E106" s="159"/>
+      <c r="C106" s="162"/>
+      <c r="D106" s="163"/>
+      <c r="E106" s="163"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5504,9 +5504,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="158"/>
-      <c r="D123" s="159"/>
-      <c r="E123" s="159"/>
+      <c r="C123" s="162"/>
+      <c r="D123" s="163"/>
+      <c r="E123" s="163"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5657,9 +5657,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="158"/>
-      <c r="D140" s="159"/>
-      <c r="E140" s="159"/>
+      <c r="C140" s="162"/>
+      <c r="D140" s="163"/>
+      <c r="E140" s="163"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5810,9 +5810,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="158"/>
-      <c r="D157" s="159"/>
-      <c r="E157" s="159"/>
+      <c r="C157" s="162"/>
+      <c r="D157" s="163"/>
+      <c r="E157" s="163"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -5963,9 +5963,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="158"/>
-      <c r="D174" s="159"/>
-      <c r="E174" s="159"/>
+      <c r="C174" s="162"/>
+      <c r="D174" s="163"/>
+      <c r="E174" s="163"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6116,9 +6116,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="158"/>
-      <c r="D191" s="159"/>
-      <c r="E191" s="159"/>
+      <c r="C191" s="162"/>
+      <c r="D191" s="163"/>
+      <c r="E191" s="163"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6269,9 +6269,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="158"/>
-      <c r="D208" s="159"/>
-      <c r="E208" s="159"/>
+      <c r="C208" s="162"/>
+      <c r="D208" s="163"/>
+      <c r="E208" s="163"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6422,9 +6422,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="158"/>
-      <c r="D225" s="159"/>
-      <c r="E225" s="159"/>
+      <c r="C225" s="162"/>
+      <c r="D225" s="163"/>
+      <c r="E225" s="163"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6575,9 +6575,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="158"/>
-      <c r="D242" s="159"/>
-      <c r="E242" s="159"/>
+      <c r="C242" s="162"/>
+      <c r="D242" s="163"/>
+      <c r="E242" s="163"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6728,9 +6728,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="158"/>
-      <c r="D259" s="159"/>
-      <c r="E259" s="159"/>
+      <c r="C259" s="162"/>
+      <c r="D259" s="163"/>
+      <c r="E259" s="163"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -6881,18 +6881,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="174"/>
-      <c r="D276" s="175"/>
-      <c r="E276" s="175"/>
+      <c r="C276" s="166"/>
+      <c r="D276" s="167"/>
+      <c r="E276" s="167"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="158"/>
-      <c r="D277" s="159"/>
-      <c r="E277" s="159"/>
+      <c r="C277" s="162"/>
+      <c r="D277" s="163"/>
+      <c r="E277" s="163"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7043,9 +7043,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="160"/>
-      <c r="D294" s="161"/>
-      <c r="E294" s="161"/>
+      <c r="C294" s="164"/>
+      <c r="D294" s="165"/>
+      <c r="E294" s="165"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7196,9 +7196,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="158"/>
-      <c r="D311" s="159"/>
-      <c r="E311" s="159"/>
+      <c r="C311" s="162"/>
+      <c r="D311" s="163"/>
+      <c r="E311" s="163"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7349,9 +7349,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="158"/>
-      <c r="D328" s="159"/>
-      <c r="E328" s="159"/>
+      <c r="C328" s="162"/>
+      <c r="D328" s="163"/>
+      <c r="E328" s="163"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7502,9 +7502,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="158"/>
-      <c r="D345" s="159"/>
-      <c r="E345" s="159"/>
+      <c r="C345" s="162"/>
+      <c r="D345" s="163"/>
+      <c r="E345" s="163"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7655,9 +7655,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="158"/>
-      <c r="D362" s="159"/>
-      <c r="E362" s="159"/>
+      <c r="C362" s="162"/>
+      <c r="D362" s="163"/>
+      <c r="E362" s="163"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7808,9 +7808,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="158"/>
-      <c r="D379" s="159"/>
-      <c r="E379" s="159"/>
+      <c r="C379" s="162"/>
+      <c r="D379" s="163"/>
+      <c r="E379" s="163"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -7961,9 +7961,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="158"/>
-      <c r="D396" s="159"/>
-      <c r="E396" s="159"/>
+      <c r="C396" s="162"/>
+      <c r="D396" s="163"/>
+      <c r="E396" s="163"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8114,9 +8114,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="158"/>
-      <c r="D413" s="159"/>
-      <c r="E413" s="159"/>
+      <c r="C413" s="162"/>
+      <c r="D413" s="163"/>
+      <c r="E413" s="163"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8267,9 +8267,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="158"/>
-      <c r="D430" s="159"/>
-      <c r="E430" s="159"/>
+      <c r="C430" s="162"/>
+      <c r="D430" s="163"/>
+      <c r="E430" s="163"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8420,9 +8420,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="158"/>
-      <c r="D447" s="159"/>
-      <c r="E447" s="159"/>
+      <c r="C447" s="162"/>
+      <c r="D447" s="163"/>
+      <c r="E447" s="163"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8573,9 +8573,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="158"/>
-      <c r="D464" s="159"/>
-      <c r="E464" s="159"/>
+      <c r="C464" s="162"/>
+      <c r="D464" s="163"/>
+      <c r="E464" s="163"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8726,9 +8726,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="158"/>
-      <c r="D481" s="159"/>
-      <c r="E481" s="159"/>
+      <c r="C481" s="162"/>
+      <c r="D481" s="163"/>
+      <c r="E481" s="163"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -8879,9 +8879,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="158"/>
-      <c r="D498" s="159"/>
-      <c r="E498" s="159"/>
+      <c r="C498" s="162"/>
+      <c r="D498" s="163"/>
+      <c r="E498" s="163"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9032,9 +9032,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="158"/>
-      <c r="D515" s="159"/>
-      <c r="E515" s="159"/>
+      <c r="C515" s="162"/>
+      <c r="D515" s="163"/>
+      <c r="E515" s="163"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9185,9 +9185,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="158"/>
-      <c r="D532" s="159"/>
-      <c r="E532" s="159"/>
+      <c r="C532" s="162"/>
+      <c r="D532" s="163"/>
+      <c r="E532" s="163"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9338,18 +9338,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="172"/>
-      <c r="D549" s="173"/>
-      <c r="E549" s="173"/>
+      <c r="C549" s="168"/>
+      <c r="D549" s="169"/>
+      <c r="E549" s="169"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="158"/>
-      <c r="D550" s="159"/>
-      <c r="E550" s="159"/>
+      <c r="C550" s="162"/>
+      <c r="D550" s="163"/>
+      <c r="E550" s="163"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9500,9 +9500,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="160"/>
-      <c r="D567" s="161"/>
-      <c r="E567" s="161"/>
+      <c r="C567" s="164"/>
+      <c r="D567" s="165"/>
+      <c r="E567" s="165"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9653,9 +9653,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="158"/>
-      <c r="D584" s="159"/>
-      <c r="E584" s="159"/>
+      <c r="C584" s="162"/>
+      <c r="D584" s="163"/>
+      <c r="E584" s="163"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9806,9 +9806,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="158"/>
-      <c r="D601" s="159"/>
-      <c r="E601" s="159"/>
+      <c r="C601" s="162"/>
+      <c r="D601" s="163"/>
+      <c r="E601" s="163"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -9959,9 +9959,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="158"/>
-      <c r="D618" s="159"/>
-      <c r="E618" s="159"/>
+      <c r="C618" s="162"/>
+      <c r="D618" s="163"/>
+      <c r="E618" s="163"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10112,9 +10112,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="158"/>
-      <c r="D635" s="159"/>
-      <c r="E635" s="159"/>
+      <c r="C635" s="162"/>
+      <c r="D635" s="163"/>
+      <c r="E635" s="163"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10265,9 +10265,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="158"/>
-      <c r="D652" s="159"/>
-      <c r="E652" s="159"/>
+      <c r="C652" s="162"/>
+      <c r="D652" s="163"/>
+      <c r="E652" s="163"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10418,9 +10418,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="158"/>
-      <c r="D669" s="159"/>
-      <c r="E669" s="159"/>
+      <c r="C669" s="162"/>
+      <c r="D669" s="163"/>
+      <c r="E669" s="163"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10571,9 +10571,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="158"/>
-      <c r="D686" s="159"/>
-      <c r="E686" s="159"/>
+      <c r="C686" s="162"/>
+      <c r="D686" s="163"/>
+      <c r="E686" s="163"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10724,9 +10724,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="158"/>
-      <c r="D703" s="159"/>
-      <c r="E703" s="159"/>
+      <c r="C703" s="162"/>
+      <c r="D703" s="163"/>
+      <c r="E703" s="163"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -10877,9 +10877,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="158"/>
-      <c r="D720" s="159"/>
-      <c r="E720" s="159"/>
+      <c r="C720" s="162"/>
+      <c r="D720" s="163"/>
+      <c r="E720" s="163"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11030,9 +11030,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="158"/>
-      <c r="D737" s="159"/>
-      <c r="E737" s="159"/>
+      <c r="C737" s="162"/>
+      <c r="D737" s="163"/>
+      <c r="E737" s="163"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11183,9 +11183,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="158"/>
-      <c r="D754" s="159"/>
-      <c r="E754" s="159"/>
+      <c r="C754" s="162"/>
+      <c r="D754" s="163"/>
+      <c r="E754" s="163"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11336,9 +11336,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="158"/>
-      <c r="D771" s="159"/>
-      <c r="E771" s="159"/>
+      <c r="C771" s="162"/>
+      <c r="D771" s="163"/>
+      <c r="E771" s="163"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11489,9 +11489,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="158"/>
-      <c r="D788" s="159"/>
-      <c r="E788" s="159"/>
+      <c r="C788" s="162"/>
+      <c r="D788" s="163"/>
+      <c r="E788" s="163"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11642,9 +11642,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="158"/>
-      <c r="D805" s="159"/>
-      <c r="E805" s="159"/>
+      <c r="C805" s="162"/>
+      <c r="D805" s="163"/>
+      <c r="E805" s="163"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11804,9 +11804,9 @@
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="158"/>
-      <c r="D823" s="159"/>
-      <c r="E823" s="159"/>
+      <c r="C823" s="162"/>
+      <c r="D823" s="163"/>
+      <c r="E823" s="163"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -11957,9 +11957,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="160"/>
-      <c r="D840" s="161"/>
-      <c r="E840" s="161"/>
+      <c r="C840" s="164"/>
+      <c r="D840" s="165"/>
+      <c r="E840" s="165"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12110,9 +12110,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="158"/>
-      <c r="D857" s="159"/>
-      <c r="E857" s="159"/>
+      <c r="C857" s="162"/>
+      <c r="D857" s="163"/>
+      <c r="E857" s="163"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12263,9 +12263,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="158"/>
-      <c r="D874" s="159"/>
-      <c r="E874" s="159"/>
+      <c r="C874" s="162"/>
+      <c r="D874" s="163"/>
+      <c r="E874" s="163"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12416,9 +12416,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="158"/>
-      <c r="D891" s="159"/>
-      <c r="E891" s="159"/>
+      <c r="C891" s="162"/>
+      <c r="D891" s="163"/>
+      <c r="E891" s="163"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12569,9 +12569,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="158"/>
-      <c r="D908" s="159"/>
-      <c r="E908" s="159"/>
+      <c r="C908" s="162"/>
+      <c r="D908" s="163"/>
+      <c r="E908" s="163"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12722,9 +12722,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="158"/>
-      <c r="D925" s="159"/>
-      <c r="E925" s="159"/>
+      <c r="C925" s="162"/>
+      <c r="D925" s="163"/>
+      <c r="E925" s="163"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -12875,9 +12875,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="158"/>
-      <c r="D942" s="159"/>
-      <c r="E942" s="159"/>
+      <c r="C942" s="162"/>
+      <c r="D942" s="163"/>
+      <c r="E942" s="163"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13028,9 +13028,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="158"/>
-      <c r="D959" s="159"/>
-      <c r="E959" s="159"/>
+      <c r="C959" s="162"/>
+      <c r="D959" s="163"/>
+      <c r="E959" s="163"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13181,9 +13181,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="158"/>
-      <c r="D976" s="159"/>
-      <c r="E976" s="159"/>
+      <c r="C976" s="162"/>
+      <c r="D976" s="163"/>
+      <c r="E976" s="163"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13334,9 +13334,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="158"/>
-      <c r="D993" s="159"/>
-      <c r="E993" s="159"/>
+      <c r="C993" s="162"/>
+      <c r="D993" s="163"/>
+      <c r="E993" s="163"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13487,9 +13487,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="158"/>
-      <c r="D1010" s="159"/>
-      <c r="E1010" s="159"/>
+      <c r="C1010" s="162"/>
+      <c r="D1010" s="163"/>
+      <c r="E1010" s="163"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13640,9 +13640,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="158"/>
-      <c r="D1027" s="159"/>
-      <c r="E1027" s="159"/>
+      <c r="C1027" s="162"/>
+      <c r="D1027" s="163"/>
+      <c r="E1027" s="163"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13793,9 +13793,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="158"/>
-      <c r="D1044" s="159"/>
-      <c r="E1044" s="159"/>
+      <c r="C1044" s="162"/>
+      <c r="D1044" s="163"/>
+      <c r="E1044" s="163"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -13946,9 +13946,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="158"/>
-      <c r="D1061" s="159"/>
-      <c r="E1061" s="159"/>
+      <c r="C1061" s="162"/>
+      <c r="D1061" s="163"/>
+      <c r="E1061" s="163"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14099,9 +14099,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="158"/>
-      <c r="D1078" s="159"/>
-      <c r="E1078" s="159"/>
+      <c r="C1078" s="162"/>
+      <c r="D1078" s="163"/>
+      <c r="E1078" s="163"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14252,18 +14252,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="168"/>
-      <c r="D1095" s="169"/>
-      <c r="E1095" s="169"/>
+      <c r="C1095" s="172"/>
+      <c r="D1095" s="173"/>
+      <c r="E1095" s="173"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="158"/>
-      <c r="D1096" s="159"/>
-      <c r="E1096" s="159"/>
+      <c r="C1096" s="162"/>
+      <c r="D1096" s="163"/>
+      <c r="E1096" s="163"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14414,9 +14414,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="160"/>
-      <c r="D1113" s="161"/>
-      <c r="E1113" s="161"/>
+      <c r="C1113" s="164"/>
+      <c r="D1113" s="165"/>
+      <c r="E1113" s="165"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14567,9 +14567,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="158"/>
-      <c r="D1130" s="159"/>
-      <c r="E1130" s="159"/>
+      <c r="C1130" s="162"/>
+      <c r="D1130" s="163"/>
+      <c r="E1130" s="163"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14720,9 +14720,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="158"/>
-      <c r="D1147" s="159"/>
-      <c r="E1147" s="159"/>
+      <c r="C1147" s="162"/>
+      <c r="D1147" s="163"/>
+      <c r="E1147" s="163"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -14873,9 +14873,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="158"/>
-      <c r="D1164" s="159"/>
-      <c r="E1164" s="159"/>
+      <c r="C1164" s="162"/>
+      <c r="D1164" s="163"/>
+      <c r="E1164" s="163"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15026,9 +15026,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="158"/>
-      <c r="D1181" s="159"/>
-      <c r="E1181" s="159"/>
+      <c r="C1181" s="162"/>
+      <c r="D1181" s="163"/>
+      <c r="E1181" s="163"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15179,9 +15179,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="158"/>
-      <c r="D1198" s="159"/>
-      <c r="E1198" s="159"/>
+      <c r="C1198" s="162"/>
+      <c r="D1198" s="163"/>
+      <c r="E1198" s="163"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15332,9 +15332,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="158"/>
-      <c r="D1215" s="159"/>
-      <c r="E1215" s="159"/>
+      <c r="C1215" s="162"/>
+      <c r="D1215" s="163"/>
+      <c r="E1215" s="163"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15485,9 +15485,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="158"/>
-      <c r="D1232" s="159"/>
-      <c r="E1232" s="159"/>
+      <c r="C1232" s="162"/>
+      <c r="D1232" s="163"/>
+      <c r="E1232" s="163"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15638,9 +15638,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="158"/>
-      <c r="D1249" s="159"/>
-      <c r="E1249" s="159"/>
+      <c r="C1249" s="162"/>
+      <c r="D1249" s="163"/>
+      <c r="E1249" s="163"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15791,9 +15791,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="158"/>
-      <c r="D1266" s="159"/>
-      <c r="E1266" s="159"/>
+      <c r="C1266" s="162"/>
+      <c r="D1266" s="163"/>
+      <c r="E1266" s="163"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -15944,9 +15944,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="158"/>
-      <c r="D1283" s="159"/>
-      <c r="E1283" s="159"/>
+      <c r="C1283" s="162"/>
+      <c r="D1283" s="163"/>
+      <c r="E1283" s="163"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16097,9 +16097,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="158"/>
-      <c r="D1300" s="159"/>
-      <c r="E1300" s="159"/>
+      <c r="C1300" s="162"/>
+      <c r="D1300" s="163"/>
+      <c r="E1300" s="163"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16250,9 +16250,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="158"/>
-      <c r="D1317" s="159"/>
-      <c r="E1317" s="159"/>
+      <c r="C1317" s="162"/>
+      <c r="D1317" s="163"/>
+      <c r="E1317" s="163"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16403,9 +16403,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="158"/>
-      <c r="D1334" s="159"/>
-      <c r="E1334" s="159"/>
+      <c r="C1334" s="162"/>
+      <c r="D1334" s="163"/>
+      <c r="E1334" s="163"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16556,9 +16556,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="158"/>
-      <c r="D1351" s="159"/>
-      <c r="E1351" s="159"/>
+      <c r="C1351" s="162"/>
+      <c r="D1351" s="163"/>
+      <c r="E1351" s="163"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16709,18 +16709,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="166"/>
-      <c r="D1368" s="167"/>
-      <c r="E1368" s="167"/>
+      <c r="C1368" s="174"/>
+      <c r="D1368" s="175"/>
+      <c r="E1368" s="175"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="158"/>
-      <c r="D1369" s="159"/>
-      <c r="E1369" s="159"/>
+      <c r="C1369" s="162"/>
+      <c r="D1369" s="163"/>
+      <c r="E1369" s="163"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -16871,9 +16871,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="160"/>
-      <c r="D1386" s="161"/>
-      <c r="E1386" s="161"/>
+      <c r="C1386" s="164"/>
+      <c r="D1386" s="165"/>
+      <c r="E1386" s="165"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17024,9 +17024,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="158"/>
-      <c r="D1403" s="159"/>
-      <c r="E1403" s="159"/>
+      <c r="C1403" s="162"/>
+      <c r="D1403" s="163"/>
+      <c r="E1403" s="163"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17177,9 +17177,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="158"/>
-      <c r="D1420" s="159"/>
-      <c r="E1420" s="159"/>
+      <c r="C1420" s="162"/>
+      <c r="D1420" s="163"/>
+      <c r="E1420" s="163"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17330,9 +17330,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="158"/>
-      <c r="D1437" s="159"/>
-      <c r="E1437" s="159"/>
+      <c r="C1437" s="162"/>
+      <c r="D1437" s="163"/>
+      <c r="E1437" s="163"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17483,9 +17483,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="158"/>
-      <c r="D1454" s="159"/>
-      <c r="E1454" s="159"/>
+      <c r="C1454" s="162"/>
+      <c r="D1454" s="163"/>
+      <c r="E1454" s="163"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17636,9 +17636,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="158"/>
-      <c r="D1471" s="159"/>
-      <c r="E1471" s="159"/>
+      <c r="C1471" s="162"/>
+      <c r="D1471" s="163"/>
+      <c r="E1471" s="163"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17789,9 +17789,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="158"/>
-      <c r="D1488" s="159"/>
-      <c r="E1488" s="159"/>
+      <c r="C1488" s="162"/>
+      <c r="D1488" s="163"/>
+      <c r="E1488" s="163"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -17942,9 +17942,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="158"/>
-      <c r="D1505" s="159"/>
-      <c r="E1505" s="159"/>
+      <c r="C1505" s="162"/>
+      <c r="D1505" s="163"/>
+      <c r="E1505" s="163"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18095,9 +18095,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="158"/>
-      <c r="D1522" s="159"/>
-      <c r="E1522" s="159"/>
+      <c r="C1522" s="162"/>
+      <c r="D1522" s="163"/>
+      <c r="E1522" s="163"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18248,9 +18248,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="158"/>
-      <c r="D1539" s="159"/>
-      <c r="E1539" s="159"/>
+      <c r="C1539" s="162"/>
+      <c r="D1539" s="163"/>
+      <c r="E1539" s="163"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18401,9 +18401,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="158"/>
-      <c r="D1556" s="159"/>
-      <c r="E1556" s="159"/>
+      <c r="C1556" s="162"/>
+      <c r="D1556" s="163"/>
+      <c r="E1556" s="163"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18554,9 +18554,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="158"/>
-      <c r="D1573" s="159"/>
-      <c r="E1573" s="159"/>
+      <c r="C1573" s="162"/>
+      <c r="D1573" s="163"/>
+      <c r="E1573" s="163"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18707,9 +18707,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="158"/>
-      <c r="D1590" s="159"/>
-      <c r="E1590" s="159"/>
+      <c r="C1590" s="162"/>
+      <c r="D1590" s="163"/>
+      <c r="E1590" s="163"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -18860,9 +18860,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="158"/>
-      <c r="D1607" s="159"/>
-      <c r="E1607" s="159"/>
+      <c r="C1607" s="162"/>
+      <c r="D1607" s="163"/>
+      <c r="E1607" s="163"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19013,9 +19013,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="158"/>
-      <c r="D1624" s="159"/>
-      <c r="E1624" s="159"/>
+      <c r="C1624" s="162"/>
+      <c r="D1624" s="163"/>
+      <c r="E1624" s="163"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19166,18 +19166,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="164"/>
-      <c r="D1641" s="165"/>
-      <c r="E1641" s="165"/>
+      <c r="C1641" s="176"/>
+      <c r="D1641" s="177"/>
+      <c r="E1641" s="177"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="158"/>
-      <c r="D1642" s="159"/>
-      <c r="E1642" s="159"/>
+      <c r="C1642" s="162"/>
+      <c r="D1642" s="163"/>
+      <c r="E1642" s="163"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19328,9 +19328,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="160"/>
-      <c r="D1659" s="161"/>
-      <c r="E1659" s="161"/>
+      <c r="C1659" s="164"/>
+      <c r="D1659" s="165"/>
+      <c r="E1659" s="165"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19481,9 +19481,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="158"/>
-      <c r="D1676" s="159"/>
-      <c r="E1676" s="159"/>
+      <c r="C1676" s="162"/>
+      <c r="D1676" s="163"/>
+      <c r="E1676" s="163"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19634,9 +19634,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="158"/>
-      <c r="D1693" s="159"/>
-      <c r="E1693" s="159"/>
+      <c r="C1693" s="162"/>
+      <c r="D1693" s="163"/>
+      <c r="E1693" s="163"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19787,9 +19787,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="158"/>
-      <c r="D1710" s="159"/>
-      <c r="E1710" s="159"/>
+      <c r="C1710" s="162"/>
+      <c r="D1710" s="163"/>
+      <c r="E1710" s="163"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -19940,9 +19940,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="158"/>
-      <c r="D1727" s="159"/>
-      <c r="E1727" s="159"/>
+      <c r="C1727" s="162"/>
+      <c r="D1727" s="163"/>
+      <c r="E1727" s="163"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20093,9 +20093,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="158"/>
-      <c r="D1744" s="159"/>
-      <c r="E1744" s="159"/>
+      <c r="C1744" s="162"/>
+      <c r="D1744" s="163"/>
+      <c r="E1744" s="163"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20246,9 +20246,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="158"/>
-      <c r="D1761" s="159"/>
-      <c r="E1761" s="159"/>
+      <c r="C1761" s="162"/>
+      <c r="D1761" s="163"/>
+      <c r="E1761" s="163"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20399,9 +20399,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="158"/>
-      <c r="D1778" s="159"/>
-      <c r="E1778" s="159"/>
+      <c r="C1778" s="162"/>
+      <c r="D1778" s="163"/>
+      <c r="E1778" s="163"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20552,9 +20552,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="158"/>
-      <c r="D1795" s="159"/>
-      <c r="E1795" s="159"/>
+      <c r="C1795" s="162"/>
+      <c r="D1795" s="163"/>
+      <c r="E1795" s="163"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20705,9 +20705,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="158"/>
-      <c r="D1812" s="159"/>
-      <c r="E1812" s="159"/>
+      <c r="C1812" s="162"/>
+      <c r="D1812" s="163"/>
+      <c r="E1812" s="163"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -20858,9 +20858,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="158"/>
-      <c r="D1829" s="159"/>
-      <c r="E1829" s="159"/>
+      <c r="C1829" s="162"/>
+      <c r="D1829" s="163"/>
+      <c r="E1829" s="163"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21011,9 +21011,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="158"/>
-      <c r="D1846" s="159"/>
-      <c r="E1846" s="159"/>
+      <c r="C1846" s="162"/>
+      <c r="D1846" s="163"/>
+      <c r="E1846" s="163"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21164,9 +21164,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="158"/>
-      <c r="D1863" s="159"/>
-      <c r="E1863" s="159"/>
+      <c r="C1863" s="162"/>
+      <c r="D1863" s="163"/>
+      <c r="E1863" s="163"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21317,9 +21317,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="158"/>
-      <c r="D1880" s="159"/>
-      <c r="E1880" s="159"/>
+      <c r="C1880" s="162"/>
+      <c r="D1880" s="163"/>
+      <c r="E1880" s="163"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21470,9 +21470,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="158"/>
-      <c r="D1897" s="159"/>
-      <c r="E1897" s="159"/>
+      <c r="C1897" s="162"/>
+      <c r="D1897" s="163"/>
+      <c r="E1897" s="163"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21623,18 +21623,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="162"/>
-      <c r="D1914" s="163"/>
-      <c r="E1914" s="163"/>
+      <c r="C1914" s="178"/>
+      <c r="D1914" s="179"/>
+      <c r="E1914" s="179"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="158"/>
-      <c r="D1915" s="159"/>
-      <c r="E1915" s="159"/>
+      <c r="C1915" s="162"/>
+      <c r="D1915" s="163"/>
+      <c r="E1915" s="163"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21785,9 +21785,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="160"/>
-      <c r="D1932" s="161"/>
-      <c r="E1932" s="161"/>
+      <c r="C1932" s="164"/>
+      <c r="D1932" s="165"/>
+      <c r="E1932" s="165"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -21938,9 +21938,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="158"/>
-      <c r="D1949" s="159"/>
-      <c r="E1949" s="159"/>
+      <c r="C1949" s="162"/>
+      <c r="D1949" s="163"/>
+      <c r="E1949" s="163"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22091,9 +22091,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="158"/>
-      <c r="D1966" s="159"/>
-      <c r="E1966" s="159"/>
+      <c r="C1966" s="162"/>
+      <c r="D1966" s="163"/>
+      <c r="E1966" s="163"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22244,9 +22244,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="158"/>
-      <c r="D1983" s="159"/>
-      <c r="E1983" s="159"/>
+      <c r="C1983" s="162"/>
+      <c r="D1983" s="163"/>
+      <c r="E1983" s="163"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22397,9 +22397,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="158"/>
-      <c r="D2000" s="159"/>
-      <c r="E2000" s="159"/>
+      <c r="C2000" s="162"/>
+      <c r="D2000" s="163"/>
+      <c r="E2000" s="163"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22550,9 +22550,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="158"/>
-      <c r="D2017" s="159"/>
-      <c r="E2017" s="159"/>
+      <c r="C2017" s="162"/>
+      <c r="D2017" s="163"/>
+      <c r="E2017" s="163"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22703,9 +22703,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="158"/>
-      <c r="D2034" s="159"/>
-      <c r="E2034" s="159"/>
+      <c r="C2034" s="162"/>
+      <c r="D2034" s="163"/>
+      <c r="E2034" s="163"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22856,9 +22856,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="158"/>
-      <c r="D2051" s="159"/>
-      <c r="E2051" s="159"/>
+      <c r="C2051" s="162"/>
+      <c r="D2051" s="163"/>
+      <c r="E2051" s="163"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23009,9 +23009,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="158"/>
-      <c r="D2068" s="159"/>
-      <c r="E2068" s="159"/>
+      <c r="C2068" s="162"/>
+      <c r="D2068" s="163"/>
+      <c r="E2068" s="163"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23162,9 +23162,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="158"/>
-      <c r="D2085" s="159"/>
-      <c r="E2085" s="159"/>
+      <c r="C2085" s="162"/>
+      <c r="D2085" s="163"/>
+      <c r="E2085" s="163"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23315,9 +23315,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="158"/>
-      <c r="D2102" s="159"/>
-      <c r="E2102" s="159"/>
+      <c r="C2102" s="162"/>
+      <c r="D2102" s="163"/>
+      <c r="E2102" s="163"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23468,9 +23468,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="158"/>
-      <c r="D2119" s="159"/>
-      <c r="E2119" s="159"/>
+      <c r="C2119" s="162"/>
+      <c r="D2119" s="163"/>
+      <c r="E2119" s="163"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23621,9 +23621,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="158"/>
-      <c r="D2136" s="159"/>
-      <c r="E2136" s="159"/>
+      <c r="C2136" s="162"/>
+      <c r="D2136" s="163"/>
+      <c r="E2136" s="163"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23774,9 +23774,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="158"/>
-      <c r="D2153" s="159"/>
-      <c r="E2153" s="159"/>
+      <c r="C2153" s="162"/>
+      <c r="D2153" s="163"/>
+      <c r="E2153" s="163"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -23927,9 +23927,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="158"/>
-      <c r="D2170" s="159"/>
-      <c r="E2170" s="159"/>
+      <c r="C2170" s="162"/>
+      <c r="D2170" s="163"/>
+      <c r="E2170" s="163"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24077,26 +24077,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24109,111 +24194,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24240,51 +24240,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="186" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="183" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="185"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="180" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="181"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="181"/>
+      <c r="K3" s="182"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -24501,19 +24501,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="179" t="s">
+      <c r="A20" s="180" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="180"/>
-      <c r="C20" s="180"/>
-      <c r="D20" s="180"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="181"/>
+      <c r="B20" s="181"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="182"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -24730,19 +24730,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="179" t="s">
+      <c r="A37" s="180" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="180"/>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="180"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="180"/>
-      <c r="K37" s="181"/>
+      <c r="B37" s="181"/>
+      <c r="C37" s="181"/>
+      <c r="D37" s="181"/>
+      <c r="E37" s="181"/>
+      <c r="F37" s="181"/>
+      <c r="G37" s="181"/>
+      <c r="H37" s="181"/>
+      <c r="I37" s="181"/>
+      <c r="J37" s="181"/>
+      <c r="K37" s="182"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25000,28 +25000,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="186"/>
+      <c r="A3" s="187"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="187"/>
+      <c r="A4" s="188"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="187"/>
+      <c r="A5" s="188"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="187"/>
+      <c r="A6" s="188"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="187"/>
+      <c r="A7" s="188"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="187"/>
+      <c r="A8" s="188"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="187"/>
+      <c r="A9" s="188"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="188"/>
+      <c r="A10" s="189"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25204,10 +25204,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="190" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="190"/>
+      <c r="C1" s="191"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25218,7 +25218,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="192" t="s">
         <v>209</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25232,19 +25232,19 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="192"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
       <c r="C4" s="132" t="str">
         <f>FrameCounts!B3</f>
-        <v>adelikat</v>
+        <v>adelikat &amp; sonikkustar</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="192"/>
+      <c r="A5" s="193"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25253,7 +25253,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="192"/>
+      <c r="A6" s="193"/>
       <c r="B6" s="139" t="s">
         <v>211</v>
       </c>
@@ -25265,7 +25265,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="192"/>
+      <c r="A7" s="193"/>
       <c r="B7" s="128" t="s">
         <v>177</v>
       </c>
@@ -25277,7 +25277,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="192"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="128" t="s">
         <v>178</v>
       </c>
@@ -25286,7 +25286,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="193"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25301,7 +25301,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="191" t="s">
+      <c r="A11" s="192" t="s">
         <v>210</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25315,7 +25315,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="192"/>
+      <c r="A12" s="193"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25327,7 +25327,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="192"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25336,7 +25336,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="192"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="139" t="s">
         <v>211</v>
       </c>
@@ -25348,7 +25348,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="192"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="128" t="s">
         <v>177</v>
       </c>
@@ -25360,7 +25360,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="192"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="128" t="s">
         <v>178</v>
       </c>
@@ -25369,7 +25369,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="193"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25384,7 +25384,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="191" t="s">
+      <c r="A19" s="192" t="s">
         <v>210</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25393,7 +25393,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="192"/>
+      <c r="A20" s="193"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25403,14 +25403,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="192"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="192"/>
+      <c r="A22" s="193"/>
       <c r="B22" s="139" t="s">
         <v>211</v>
       </c>
@@ -25420,7 +25420,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="192"/>
+      <c r="A23" s="193"/>
       <c r="B23" s="128" t="s">
         <v>177</v>
       </c>
@@ -25430,14 +25430,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="192"/>
+      <c r="A24" s="193"/>
       <c r="B24" s="128" t="s">
         <v>178</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="193"/>
+      <c r="A25" s="194"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25472,163 +25472,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="205" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="206"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="200" t="s">
+      <c r="A2" s="211" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="201"/>
+      <c r="B2" s="212"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="213" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="201"/>
+      <c r="B3" s="212"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
+      <c r="A4" s="209"/>
+      <c r="B4" s="210"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="205" t="s">
+      <c r="A5" s="207" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="206"/>
+      <c r="B5" s="208"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="211" t="s">
+      <c r="A7" s="199" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="212"/>
+      <c r="B7" s="200"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="209" t="s">
+      <c r="A9" s="201" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="210"/>
+      <c r="B9" s="202"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="196"/>
-      <c r="B10" s="197"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="195" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="199"/>
+      <c r="B11" s="196"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="198" t="s">
+      <c r="A12" s="195" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="199"/>
+      <c r="B12" s="196"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="195" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="199"/>
+      <c r="B13" s="196"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="198" t="s">
+      <c r="A14" s="195" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="199"/>
+      <c r="B14" s="196"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="198" t="s">
+      <c r="A15" s="195" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="199"/>
+      <c r="B15" s="196"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="198" t="s">
+      <c r="A16" s="195" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="199"/>
+      <c r="B16" s="196"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="194" t="s">
+      <c r="A17" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="195"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="211" t="s">
+      <c r="A19" s="199" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="212"/>
+      <c r="B19" s="200"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="209" t="s">
+      <c r="A21" s="201" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="210"/>
+      <c r="B21" s="202"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="196"/>
-      <c r="B22" s="197"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="204"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="198" t="s">
+      <c r="A23" s="195" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="199"/>
+      <c r="B23" s="196"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="198"/>
-      <c r="B24" s="199"/>
+      <c r="A24" s="195"/>
+      <c r="B24" s="196"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="198" t="s">
+      <c r="A25" s="195" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="199"/>
+      <c r="B25" s="196"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="198" t="s">
+      <c r="A26" s="195" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="199"/>
+      <c r="B26" s="196"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="194"/>
-      <c r="B27" s="195"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25639,6 +25626,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Spiderman2 - rescue hostage 4 frames faster, using a different idea for the last fire room right before.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -2000,6 +2000,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2021,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2079,20 +2083,34 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2102,24 +2120,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,8 +2430,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2447,16 +2447,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="157" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="156" t="s">
+      <c r="B1" s="156"/>
+      <c r="C1" s="158" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="157"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65538)</f>
@@ -2534,10 +2534,10 @@
       <c r="B5" s="147" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="155"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2553,10 +2553,10 @@
       <c r="B6" s="147" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="155" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="156"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2574,7 +2574,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="160" t="s">
         <v>187</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="151"/>
+      <c r="A9" s="153"/>
       <c r="B9" s="98" t="s">
         <v>183</v>
       </c>
@@ -2608,7 +2608,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="151"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="148" t="s">
         <v>212</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="151"/>
+      <c r="A11" s="153"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2644,7 +2644,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="151"/>
+      <c r="A12" s="153"/>
       <c r="B12" s="148" t="s">
         <v>218</v>
       </c>
@@ -2659,7 +2659,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="151"/>
+      <c r="A13" s="153"/>
       <c r="B13" s="148" t="s">
         <v>219</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="151"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="148" t="s">
         <v>220</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="151"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="148" t="s">
         <v>221</v>
       </c>
@@ -2704,7 +2704,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A16" s="151"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="98" t="s">
         <v>186</v>
       </c>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="18" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="154" t="s">
         <v>222</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2767,7 +2767,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="151"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="98" t="s">
         <v>183</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A21" s="151"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="148" t="s">
         <v>221</v>
       </c>
@@ -2804,7 +2804,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A22" s="151"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="149" t="s">
         <v>223</v>
       </c>
@@ -2821,21 +2821,21 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:8" outlineLevel="1">
-      <c r="A23" s="151"/>
-      <c r="B23" s="215" t="s">
+      <c r="A23" s="153"/>
+      <c r="B23" s="151" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="215"/>
-      <c r="D23" s="215"/>
-      <c r="E23" s="215">
+      <c r="C23" s="151"/>
+      <c r="D23" s="151"/>
+      <c r="E23" s="151">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23" s="215"/>
+      <c r="F23" s="151"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="151"/>
-      <c r="B24" s="214" t="s">
+      <c r="A24" s="153"/>
+      <c r="B24" s="150" t="s">
         <v>221</v>
       </c>
       <c r="C24" s="101"/>
@@ -2849,23 +2849,25 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="151"/>
-      <c r="B25" s="214" t="s">
+      <c r="A25" s="153"/>
+      <c r="B25" s="150" t="s">
         <v>226</v>
       </c>
-      <c r="C25" s="101"/>
+      <c r="C25" s="101">
+        <v>2181</v>
+      </c>
       <c r="D25" s="101">
         <v>2227</v>
       </c>
       <c r="E25" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="151"/>
-      <c r="B26" s="214" t="s">
+      <c r="A26" s="153"/>
+      <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
       <c r="C26" s="101"/>
@@ -2879,8 +2881,8 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="151"/>
-      <c r="B27" s="214" t="s">
+      <c r="A27" s="153"/>
+      <c r="B27" s="150" t="s">
         <v>229</v>
       </c>
       <c r="C27" s="101"/>
@@ -2894,8 +2896,8 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="151"/>
-      <c r="B28" s="214" t="s">
+      <c r="A28" s="153"/>
+      <c r="B28" s="150" t="s">
         <v>230</v>
       </c>
       <c r="C28" s="101"/>
@@ -2909,8 +2911,8 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="151"/>
-      <c r="B29" s="214" t="s">
+      <c r="A29" s="153"/>
+      <c r="B29" s="150" t="s">
         <v>231</v>
       </c>
       <c r="C29" s="101"/>
@@ -2924,8 +2926,8 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="151"/>
-      <c r="B30" s="214" t="s">
+      <c r="A30" s="153"/>
+      <c r="B30" s="150" t="s">
         <v>232</v>
       </c>
       <c r="C30" s="101"/>
@@ -2939,21 +2941,21 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:8" outlineLevel="1">
-      <c r="A31" s="151"/>
-      <c r="B31" s="215" t="s">
+      <c r="A31" s="153"/>
+      <c r="B31" s="151" t="s">
         <v>233</v>
       </c>
-      <c r="C31" s="215"/>
-      <c r="D31" s="215"/>
-      <c r="E31" s="215">
+      <c r="C31" s="151"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="151">
         <f t="shared" ref="E31" si="2">IF(AND(C31&gt;0,D31&gt;0), D31-C31, 0)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="215"/>
+      <c r="F31" s="151"/>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="151"/>
-      <c r="B32" s="214" t="s">
+      <c r="A32" s="153"/>
+      <c r="B32" s="150" t="s">
         <v>221</v>
       </c>
       <c r="C32" s="101"/>
@@ -2967,8 +2969,8 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A33" s="151"/>
-      <c r="B33" s="214" t="s">
+      <c r="A33" s="153"/>
+      <c r="B33" s="150" t="s">
         <v>234</v>
       </c>
       <c r="C33" s="101"/>
@@ -2982,8 +2984,8 @@
       <c r="F33" s="105"/>
     </row>
     <row r="34" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A34" s="151"/>
-      <c r="B34" s="214" t="s">
+      <c r="A34" s="153"/>
+      <c r="B34" s="150" t="s">
         <v>168</v>
       </c>
       <c r="C34" s="101"/>
@@ -2997,8 +2999,8 @@
       <c r="F34" s="105"/>
     </row>
     <row r="35" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A35" s="151"/>
-      <c r="B35" s="214" t="s">
+      <c r="A35" s="153"/>
+      <c r="B35" s="150" t="s">
         <v>235</v>
       </c>
       <c r="C35" s="101"/>
@@ -3012,7 +3014,7 @@
       <c r="F35" s="105"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A36" s="151"/>
+      <c r="A36" s="153"/>
       <c r="B36" s="98" t="s">
         <v>186</v>
       </c>
@@ -3053,7 +3055,7 @@
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="39" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A39" s="150" t="s">
+      <c r="A39" s="152" t="s">
         <v>169</v>
       </c>
       <c r="B39" s="113" t="s">
@@ -3073,7 +3075,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="151"/>
+      <c r="A40" s="153"/>
       <c r="B40" s="98" t="s">
         <v>183</v>
       </c>
@@ -3088,8 +3090,8 @@
       <c r="F40" s="104"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A41" s="151"/>
-      <c r="B41" s="214" t="s">
+      <c r="A41" s="153"/>
+      <c r="B41" s="150" t="s">
         <v>221</v>
       </c>
       <c r="C41" s="101"/>
@@ -3103,7 +3105,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A42" s="151"/>
+      <c r="A42" s="153"/>
       <c r="B42" s="100"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -3114,7 +3116,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A43" s="151"/>
+      <c r="A43" s="153"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3125,7 +3127,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A44" s="151"/>
+      <c r="A44" s="153"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3136,7 +3138,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A45" s="151"/>
+      <c r="A45" s="153"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3147,7 +3149,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A46" s="151"/>
+      <c r="A46" s="153"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3158,7 +3160,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A47" s="151"/>
+      <c r="A47" s="153"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3169,7 +3171,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A48" s="151"/>
+      <c r="A48" s="153"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3180,7 +3182,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="151"/>
+      <c r="A49" s="153"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3191,7 +3193,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A50" s="151"/>
+      <c r="A50" s="153"/>
       <c r="B50" s="100"/>
       <c r="C50" s="101"/>
       <c r="D50" s="101"/>
@@ -3202,7 +3204,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A51" s="151"/>
+      <c r="A51" s="153"/>
       <c r="B51" s="100"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
@@ -3213,7 +3215,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A52" s="151"/>
+      <c r="A52" s="153"/>
       <c r="B52" s="100"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
@@ -3224,7 +3226,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A53" s="151"/>
+      <c r="A53" s="153"/>
       <c r="B53" s="98" t="s">
         <v>186</v>
       </c>
@@ -3263,7 +3265,7 @@
     </row>
     <row r="55" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="56" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A56" s="152" t="s">
+      <c r="A56" s="154" t="s">
         <v>170</v>
       </c>
       <c r="B56" s="109" t="s">
@@ -3283,7 +3285,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A57" s="151"/>
+      <c r="A57" s="153"/>
       <c r="B57" s="98" t="s">
         <v>183</v>
       </c>
@@ -3296,7 +3298,7 @@
       <c r="F57" s="104"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A58" s="151"/>
+      <c r="A58" s="153"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3307,7 +3309,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A59" s="151"/>
+      <c r="A59" s="153"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3318,7 +3320,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A60" s="151"/>
+      <c r="A60" s="153"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3329,7 +3331,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A61" s="151"/>
+      <c r="A61" s="153"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3340,7 +3342,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A62" s="151"/>
+      <c r="A62" s="153"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3351,7 +3353,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A63" s="151"/>
+      <c r="A63" s="153"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3362,7 +3364,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A64" s="151"/>
+      <c r="A64" s="153"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3373,7 +3375,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A65" s="151"/>
+      <c r="A65" s="153"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3384,7 +3386,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A66" s="151"/>
+      <c r="A66" s="153"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3395,7 +3397,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A67" s="151"/>
+      <c r="A67" s="153"/>
       <c r="B67" s="100"/>
       <c r="C67" s="101"/>
       <c r="D67" s="101"/>
@@ -3406,7 +3408,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A68" s="151"/>
+      <c r="A68" s="153"/>
       <c r="B68" s="100"/>
       <c r="C68" s="101"/>
       <c r="D68" s="101"/>
@@ -3417,7 +3419,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A69" s="151"/>
+      <c r="A69" s="153"/>
       <c r="B69" s="100"/>
       <c r="C69" s="101"/>
       <c r="D69" s="101"/>
@@ -3428,7 +3430,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A70" s="151"/>
+      <c r="A70" s="153"/>
       <c r="B70" s="98" t="s">
         <v>186</v>
       </c>
@@ -3467,7 +3469,7 @@
     </row>
     <row r="72" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="73" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A73" s="150" t="s">
+      <c r="A73" s="152" t="s">
         <v>171</v>
       </c>
       <c r="B73" s="113" t="s">
@@ -3487,7 +3489,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A74" s="151"/>
+      <c r="A74" s="153"/>
       <c r="B74" s="98" t="s">
         <v>183</v>
       </c>
@@ -3500,7 +3502,7 @@
       <c r="F74" s="104"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A75" s="151"/>
+      <c r="A75" s="153"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3511,7 +3513,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A76" s="151"/>
+      <c r="A76" s="153"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3522,7 +3524,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A77" s="151"/>
+      <c r="A77" s="153"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3533,7 +3535,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A78" s="151"/>
+      <c r="A78" s="153"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3544,7 +3546,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A79" s="151"/>
+      <c r="A79" s="153"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3555,7 +3557,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A80" s="151"/>
+      <c r="A80" s="153"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3566,7 +3568,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A81" s="151"/>
+      <c r="A81" s="153"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3577,7 +3579,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A82" s="151"/>
+      <c r="A82" s="153"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3588,7 +3590,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A83" s="151"/>
+      <c r="A83" s="153"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3599,7 +3601,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A84" s="151"/>
+      <c r="A84" s="153"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3610,7 +3612,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A85" s="151"/>
+      <c r="A85" s="153"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3621,7 +3623,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A86" s="151"/>
+      <c r="A86" s="153"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3632,7 +3634,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A87" s="151"/>
+      <c r="A87" s="153"/>
       <c r="B87" s="98" t="s">
         <v>186</v>
       </c>
@@ -3671,7 +3673,7 @@
     </row>
     <row r="89" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="90" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A90" s="152" t="s">
+      <c r="A90" s="154" t="s">
         <v>172</v>
       </c>
       <c r="B90" s="109" t="s">
@@ -3691,7 +3693,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A91" s="151"/>
+      <c r="A91" s="153"/>
       <c r="B91" s="98" t="s">
         <v>183</v>
       </c>
@@ -3704,7 +3706,7 @@
       <c r="F91" s="104"/>
     </row>
     <row r="92" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A92" s="151"/>
+      <c r="A92" s="153"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3715,7 +3717,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A93" s="151"/>
+      <c r="A93" s="153"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3726,7 +3728,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A94" s="151"/>
+      <c r="A94" s="153"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3737,7 +3739,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A95" s="151"/>
+      <c r="A95" s="153"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3748,7 +3750,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A96" s="151"/>
+      <c r="A96" s="153"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3759,7 +3761,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A97" s="151"/>
+      <c r="A97" s="153"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3770,7 +3772,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A98" s="151"/>
+      <c r="A98" s="153"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3781,7 +3783,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A99" s="151"/>
+      <c r="A99" s="153"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3792,7 +3794,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A100" s="151"/>
+      <c r="A100" s="153"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3803,7 +3805,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A101" s="151"/>
+      <c r="A101" s="153"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3814,7 +3816,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A102" s="151"/>
+      <c r="A102" s="153"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3825,7 +3827,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A103" s="151"/>
+      <c r="A103" s="153"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3836,7 +3838,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A104" s="151"/>
+      <c r="A104" s="153"/>
       <c r="B104" s="98" t="s">
         <v>186</v>
       </c>
@@ -3874,7 +3876,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A107" s="150" t="s">
+      <c r="A107" s="152" t="s">
         <v>173</v>
       </c>
       <c r="B107" s="113" t="s">
@@ -3894,7 +3896,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A108" s="151"/>
+      <c r="A108" s="153"/>
       <c r="B108" s="98" t="s">
         <v>183</v>
       </c>
@@ -3907,7 +3909,7 @@
       <c r="F108" s="104"/>
     </row>
     <row r="109" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A109" s="151"/>
+      <c r="A109" s="153"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3918,7 +3920,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A110" s="151"/>
+      <c r="A110" s="153"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3929,7 +3931,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A111" s="151"/>
+      <c r="A111" s="153"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3940,7 +3942,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A112" s="151"/>
+      <c r="A112" s="153"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3951,7 +3953,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A113" s="151"/>
+      <c r="A113" s="153"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3962,7 +3964,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A114" s="151"/>
+      <c r="A114" s="153"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3973,7 +3975,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A115" s="151"/>
+      <c r="A115" s="153"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3984,7 +3986,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A116" s="151"/>
+      <c r="A116" s="153"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3995,7 +3997,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A117" s="151"/>
+      <c r="A117" s="153"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4006,7 +4008,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A118" s="151"/>
+      <c r="A118" s="153"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4017,7 +4019,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A119" s="151"/>
+      <c r="A119" s="153"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4028,7 +4030,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A120" s="151"/>
+      <c r="A120" s="153"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4039,7 +4041,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A121" s="151"/>
+      <c r="A121" s="153"/>
       <c r="B121" s="98" t="s">
         <v>186</v>
       </c>
@@ -4077,7 +4079,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A124" s="152" t="s">
+      <c r="A124" s="154" t="s">
         <v>174</v>
       </c>
       <c r="B124" s="109" t="s">
@@ -4097,7 +4099,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A125" s="151"/>
+      <c r="A125" s="153"/>
       <c r="B125" s="98" t="s">
         <v>183</v>
       </c>
@@ -4110,7 +4112,7 @@
       <c r="F125" s="104"/>
     </row>
     <row r="126" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A126" s="151"/>
+      <c r="A126" s="153"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4121,7 +4123,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A127" s="151"/>
+      <c r="A127" s="153"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4132,7 +4134,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A128" s="151"/>
+      <c r="A128" s="153"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4143,7 +4145,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A129" s="151"/>
+      <c r="A129" s="153"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4154,7 +4156,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A130" s="151"/>
+      <c r="A130" s="153"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4165,7 +4167,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A131" s="151"/>
+      <c r="A131" s="153"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4176,7 +4178,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A132" s="151"/>
+      <c r="A132" s="153"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4187,7 +4189,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A133" s="151"/>
+      <c r="A133" s="153"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4198,7 +4200,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A134" s="151"/>
+      <c r="A134" s="153"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4209,7 +4211,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A135" s="151"/>
+      <c r="A135" s="153"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4220,7 +4222,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A136" s="151"/>
+      <c r="A136" s="153"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4231,7 +4233,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A137" s="151"/>
+      <c r="A137" s="153"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4242,7 +4244,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A138" s="151"/>
+      <c r="A138" s="153"/>
       <c r="B138" s="98" t="s">
         <v>186</v>
       </c>
@@ -4280,7 +4282,7 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A141" s="150" t="s">
+      <c r="A141" s="152" t="s">
         <v>175</v>
       </c>
       <c r="B141" s="113" t="s">
@@ -4300,7 +4302,7 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A142" s="151"/>
+      <c r="A142" s="153"/>
       <c r="B142" s="98" t="s">
         <v>183</v>
       </c>
@@ -4313,7 +4315,7 @@
       <c r="F142" s="104"/>
     </row>
     <row r="143" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A143" s="151"/>
+      <c r="A143" s="153"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4324,7 +4326,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A144" s="151"/>
+      <c r="A144" s="153"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4335,7 +4337,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A145" s="151"/>
+      <c r="A145" s="153"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4346,7 +4348,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="151"/>
+      <c r="A146" s="153"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4357,7 +4359,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="151"/>
+      <c r="A147" s="153"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4368,7 +4370,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="151"/>
+      <c r="A148" s="153"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4379,7 +4381,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="151"/>
+      <c r="A149" s="153"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4390,7 +4392,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="151"/>
+      <c r="A150" s="153"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4401,7 +4403,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="151"/>
+      <c r="A151" s="153"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4412,7 +4414,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="151"/>
+      <c r="A152" s="153"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4423,7 +4425,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="151"/>
+      <c r="A153" s="153"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4434,7 +4436,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="151"/>
+      <c r="A154" s="153"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4445,7 +4447,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A155" s="151"/>
+      <c r="A155" s="153"/>
       <c r="B155" s="98" t="s">
         <v>186</v>
       </c>
@@ -4484,6 +4486,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4492,11 +4499,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4528,13 +4530,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4564,18 +4566,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4727,9 +4729,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="162"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4880,9 +4882,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5033,9 +5035,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="159"/>
-      <c r="D55" s="160"/>
-      <c r="E55" s="160"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5186,9 +5188,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="159"/>
-      <c r="D72" s="160"/>
-      <c r="E72" s="160"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5339,9 +5341,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="159"/>
-      <c r="D89" s="160"/>
-      <c r="E89" s="160"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5492,9 +5494,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="159"/>
-      <c r="D106" s="160"/>
-      <c r="E106" s="160"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5645,9 +5647,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="159"/>
-      <c r="D123" s="160"/>
-      <c r="E123" s="160"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5798,9 +5800,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="159"/>
-      <c r="D140" s="160"/>
-      <c r="E140" s="160"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5951,9 +5953,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="159"/>
-      <c r="D157" s="160"/>
-      <c r="E157" s="160"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6104,9 +6106,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="159"/>
-      <c r="D174" s="160"/>
-      <c r="E174" s="160"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6257,9 +6259,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="159"/>
-      <c r="D191" s="160"/>
-      <c r="E191" s="160"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6410,9 +6412,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="159"/>
-      <c r="D208" s="160"/>
-      <c r="E208" s="160"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6563,9 +6565,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="159"/>
-      <c r="D225" s="160"/>
-      <c r="E225" s="160"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6716,9 +6718,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="159"/>
-      <c r="D242" s="160"/>
-      <c r="E242" s="160"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6869,9 +6871,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="159"/>
-      <c r="D259" s="160"/>
-      <c r="E259" s="160"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7022,18 +7024,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="175"/>
-      <c r="D276" s="176"/>
-      <c r="E276" s="176"/>
+      <c r="C276" s="168"/>
+      <c r="D276" s="169"/>
+      <c r="E276" s="169"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="159"/>
-      <c r="D277" s="160"/>
-      <c r="E277" s="160"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7184,9 +7186,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="161"/>
-      <c r="D294" s="162"/>
-      <c r="E294" s="162"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7337,9 +7339,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="159"/>
-      <c r="D311" s="160"/>
-      <c r="E311" s="160"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7490,9 +7492,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="159"/>
-      <c r="D328" s="160"/>
-      <c r="E328" s="160"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7643,9 +7645,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="159"/>
-      <c r="D345" s="160"/>
-      <c r="E345" s="160"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7796,9 +7798,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="159"/>
-      <c r="D362" s="160"/>
-      <c r="E362" s="160"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7949,9 +7951,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="159"/>
-      <c r="D379" s="160"/>
-      <c r="E379" s="160"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8102,9 +8104,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="159"/>
-      <c r="D396" s="160"/>
-      <c r="E396" s="160"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8255,9 +8257,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="159"/>
-      <c r="D413" s="160"/>
-      <c r="E413" s="160"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8408,9 +8410,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="159"/>
-      <c r="D430" s="160"/>
-      <c r="E430" s="160"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8561,9 +8563,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="159"/>
-      <c r="D447" s="160"/>
-      <c r="E447" s="160"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8714,9 +8716,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="159"/>
-      <c r="D464" s="160"/>
-      <c r="E464" s="160"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8867,9 +8869,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="159"/>
-      <c r="D481" s="160"/>
-      <c r="E481" s="160"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9020,9 +9022,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="159"/>
-      <c r="D498" s="160"/>
-      <c r="E498" s="160"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9173,9 +9175,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="159"/>
-      <c r="D515" s="160"/>
-      <c r="E515" s="160"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9326,9 +9328,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="159"/>
-      <c r="D532" s="160"/>
-      <c r="E532" s="160"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9479,18 +9481,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="173"/>
-      <c r="D549" s="174"/>
-      <c r="E549" s="174"/>
+      <c r="C549" s="170"/>
+      <c r="D549" s="171"/>
+      <c r="E549" s="171"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="159"/>
-      <c r="D550" s="160"/>
-      <c r="E550" s="160"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9641,9 +9643,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="161"/>
-      <c r="D567" s="162"/>
-      <c r="E567" s="162"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9794,9 +9796,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="159"/>
-      <c r="D584" s="160"/>
-      <c r="E584" s="160"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9947,9 +9949,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="159"/>
-      <c r="D601" s="160"/>
-      <c r="E601" s="160"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10100,9 +10102,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="159"/>
-      <c r="D618" s="160"/>
-      <c r="E618" s="160"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10253,9 +10255,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="159"/>
-      <c r="D635" s="160"/>
-      <c r="E635" s="160"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10406,9 +10408,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="159"/>
-      <c r="D652" s="160"/>
-      <c r="E652" s="160"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10559,9 +10561,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="159"/>
-      <c r="D669" s="160"/>
-      <c r="E669" s="160"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10712,9 +10714,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="159"/>
-      <c r="D686" s="160"/>
-      <c r="E686" s="160"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10865,9 +10867,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="159"/>
-      <c r="D703" s="160"/>
-      <c r="E703" s="160"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11018,9 +11020,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="159"/>
-      <c r="D720" s="160"/>
-      <c r="E720" s="160"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11171,9 +11173,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="159"/>
-      <c r="D737" s="160"/>
-      <c r="E737" s="160"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11324,9 +11326,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="159"/>
-      <c r="D754" s="160"/>
-      <c r="E754" s="160"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11477,9 +11479,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="159"/>
-      <c r="D771" s="160"/>
-      <c r="E771" s="160"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11630,9 +11632,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="159"/>
-      <c r="D788" s="160"/>
-      <c r="E788" s="160"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11783,9 +11785,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="159"/>
-      <c r="D805" s="160"/>
-      <c r="E805" s="160"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11936,18 +11938,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="171"/>
-      <c r="D822" s="172"/>
-      <c r="E822" s="172"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="159"/>
-      <c r="D823" s="160"/>
-      <c r="E823" s="160"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12098,9 +12100,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="161"/>
-      <c r="D840" s="162"/>
-      <c r="E840" s="162"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12251,9 +12253,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="159"/>
-      <c r="D857" s="160"/>
-      <c r="E857" s="160"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12404,9 +12406,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="159"/>
-      <c r="D874" s="160"/>
-      <c r="E874" s="160"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12557,9 +12559,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="159"/>
-      <c r="D891" s="160"/>
-      <c r="E891" s="160"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12710,9 +12712,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="159"/>
-      <c r="D908" s="160"/>
-      <c r="E908" s="160"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12863,9 +12865,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="159"/>
-      <c r="D925" s="160"/>
-      <c r="E925" s="160"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13016,9 +13018,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="159"/>
-      <c r="D942" s="160"/>
-      <c r="E942" s="160"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13169,9 +13171,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="159"/>
-      <c r="D959" s="160"/>
-      <c r="E959" s="160"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13322,9 +13324,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="159"/>
-      <c r="D976" s="160"/>
-      <c r="E976" s="160"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13475,9 +13477,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="159"/>
-      <c r="D993" s="160"/>
-      <c r="E993" s="160"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13628,9 +13630,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="159"/>
-      <c r="D1010" s="160"/>
-      <c r="E1010" s="160"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13781,9 +13783,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="159"/>
-      <c r="D1027" s="160"/>
-      <c r="E1027" s="160"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13934,9 +13936,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="159"/>
-      <c r="D1044" s="160"/>
-      <c r="E1044" s="160"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14087,9 +14089,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="159"/>
-      <c r="D1061" s="160"/>
-      <c r="E1061" s="160"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14240,9 +14242,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="159"/>
-      <c r="D1078" s="160"/>
-      <c r="E1078" s="160"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14393,18 +14395,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="169"/>
-      <c r="D1095" s="170"/>
-      <c r="E1095" s="170"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="159"/>
-      <c r="D1096" s="160"/>
-      <c r="E1096" s="160"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14555,9 +14557,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="161"/>
-      <c r="D1113" s="162"/>
-      <c r="E1113" s="162"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14708,9 +14710,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="159"/>
-      <c r="D1130" s="160"/>
-      <c r="E1130" s="160"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14861,9 +14863,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="159"/>
-      <c r="D1147" s="160"/>
-      <c r="E1147" s="160"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15014,9 +15016,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="159"/>
-      <c r="D1164" s="160"/>
-      <c r="E1164" s="160"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15167,9 +15169,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="159"/>
-      <c r="D1181" s="160"/>
-      <c r="E1181" s="160"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15320,9 +15322,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="159"/>
-      <c r="D1198" s="160"/>
-      <c r="E1198" s="160"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15473,9 +15475,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="159"/>
-      <c r="D1215" s="160"/>
-      <c r="E1215" s="160"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15626,9 +15628,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="159"/>
-      <c r="D1232" s="160"/>
-      <c r="E1232" s="160"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15779,9 +15781,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="159"/>
-      <c r="D1249" s="160"/>
-      <c r="E1249" s="160"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15932,9 +15934,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="159"/>
-      <c r="D1266" s="160"/>
-      <c r="E1266" s="160"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16085,9 +16087,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="159"/>
-      <c r="D1283" s="160"/>
-      <c r="E1283" s="160"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16238,9 +16240,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="159"/>
-      <c r="D1300" s="160"/>
-      <c r="E1300" s="160"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16391,9 +16393,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="159"/>
-      <c r="D1317" s="160"/>
-      <c r="E1317" s="160"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16544,9 +16546,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="159"/>
-      <c r="D1334" s="160"/>
-      <c r="E1334" s="160"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16697,9 +16699,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="159"/>
-      <c r="D1351" s="160"/>
-      <c r="E1351" s="160"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16850,18 +16852,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="167"/>
-      <c r="D1368" s="168"/>
-      <c r="E1368" s="168"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="159"/>
-      <c r="D1369" s="160"/>
-      <c r="E1369" s="160"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17012,9 +17014,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="161"/>
-      <c r="D1386" s="162"/>
-      <c r="E1386" s="162"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17165,9 +17167,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="159"/>
-      <c r="D1403" s="160"/>
-      <c r="E1403" s="160"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17318,9 +17320,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="159"/>
-      <c r="D1420" s="160"/>
-      <c r="E1420" s="160"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17471,9 +17473,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="159"/>
-      <c r="D1437" s="160"/>
-      <c r="E1437" s="160"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17624,9 +17626,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="159"/>
-      <c r="D1454" s="160"/>
-      <c r="E1454" s="160"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17777,9 +17779,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="159"/>
-      <c r="D1471" s="160"/>
-      <c r="E1471" s="160"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17930,9 +17932,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="159"/>
-      <c r="D1488" s="160"/>
-      <c r="E1488" s="160"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18083,9 +18085,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="159"/>
-      <c r="D1505" s="160"/>
-      <c r="E1505" s="160"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18236,9 +18238,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="159"/>
-      <c r="D1522" s="160"/>
-      <c r="E1522" s="160"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18389,9 +18391,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="159"/>
-      <c r="D1539" s="160"/>
-      <c r="E1539" s="160"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18542,9 +18544,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="159"/>
-      <c r="D1556" s="160"/>
-      <c r="E1556" s="160"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18695,9 +18697,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="159"/>
-      <c r="D1573" s="160"/>
-      <c r="E1573" s="160"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18848,9 +18850,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="159"/>
-      <c r="D1590" s="160"/>
-      <c r="E1590" s="160"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19001,9 +19003,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="159"/>
-      <c r="D1607" s="160"/>
-      <c r="E1607" s="160"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19154,9 +19156,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="159"/>
-      <c r="D1624" s="160"/>
-      <c r="E1624" s="160"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19307,18 +19309,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="165"/>
-      <c r="D1641" s="166"/>
-      <c r="E1641" s="166"/>
+      <c r="C1641" s="178"/>
+      <c r="D1641" s="179"/>
+      <c r="E1641" s="179"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="159"/>
-      <c r="D1642" s="160"/>
-      <c r="E1642" s="160"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19469,9 +19471,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="161"/>
-      <c r="D1659" s="162"/>
-      <c r="E1659" s="162"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19622,9 +19624,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="159"/>
-      <c r="D1676" s="160"/>
-      <c r="E1676" s="160"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19775,9 +19777,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="159"/>
-      <c r="D1693" s="160"/>
-      <c r="E1693" s="160"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19928,9 +19930,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="159"/>
-      <c r="D1710" s="160"/>
-      <c r="E1710" s="160"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20081,9 +20083,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="159"/>
-      <c r="D1727" s="160"/>
-      <c r="E1727" s="160"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20234,9 +20236,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="159"/>
-      <c r="D1744" s="160"/>
-      <c r="E1744" s="160"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20387,9 +20389,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="159"/>
-      <c r="D1761" s="160"/>
-      <c r="E1761" s="160"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20540,9 +20542,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="159"/>
-      <c r="D1778" s="160"/>
-      <c r="E1778" s="160"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20693,9 +20695,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="159"/>
-      <c r="D1795" s="160"/>
-      <c r="E1795" s="160"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20846,9 +20848,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="159"/>
-      <c r="D1812" s="160"/>
-      <c r="E1812" s="160"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -20999,9 +21001,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="159"/>
-      <c r="D1829" s="160"/>
-      <c r="E1829" s="160"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21152,9 +21154,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="159"/>
-      <c r="D1846" s="160"/>
-      <c r="E1846" s="160"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21305,9 +21307,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="159"/>
-      <c r="D1863" s="160"/>
-      <c r="E1863" s="160"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21458,9 +21460,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="159"/>
-      <c r="D1880" s="160"/>
-      <c r="E1880" s="160"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21611,9 +21613,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="159"/>
-      <c r="D1897" s="160"/>
-      <c r="E1897" s="160"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21764,18 +21766,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="163"/>
-      <c r="D1914" s="164"/>
-      <c r="E1914" s="164"/>
+      <c r="C1914" s="180"/>
+      <c r="D1914" s="181"/>
+      <c r="E1914" s="181"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="159"/>
-      <c r="D1915" s="160"/>
-      <c r="E1915" s="160"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21926,9 +21928,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="161"/>
-      <c r="D1932" s="162"/>
-      <c r="E1932" s="162"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22079,9 +22081,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="159"/>
-      <c r="D1949" s="160"/>
-      <c r="E1949" s="160"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22232,9 +22234,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="159"/>
-      <c r="D1966" s="160"/>
-      <c r="E1966" s="160"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22385,9 +22387,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="159"/>
-      <c r="D1983" s="160"/>
-      <c r="E1983" s="160"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22538,9 +22540,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="159"/>
-      <c r="D2000" s="160"/>
-      <c r="E2000" s="160"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22691,9 +22693,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="159"/>
-      <c r="D2017" s="160"/>
-      <c r="E2017" s="160"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22844,9 +22846,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="159"/>
-      <c r="D2034" s="160"/>
-      <c r="E2034" s="160"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22997,9 +22999,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="159"/>
-      <c r="D2051" s="160"/>
-      <c r="E2051" s="160"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23150,9 +23152,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="159"/>
-      <c r="D2068" s="160"/>
-      <c r="E2068" s="160"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23303,9 +23305,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="159"/>
-      <c r="D2085" s="160"/>
-      <c r="E2085" s="160"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23456,9 +23458,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="159"/>
-      <c r="D2102" s="160"/>
-      <c r="E2102" s="160"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23609,9 +23611,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="159"/>
-      <c r="D2119" s="160"/>
-      <c r="E2119" s="160"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23762,9 +23764,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="159"/>
-      <c r="D2136" s="160"/>
-      <c r="E2136" s="160"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23915,9 +23917,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="159"/>
-      <c r="D2153" s="160"/>
-      <c r="E2153" s="160"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24068,9 +24070,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="159"/>
-      <c r="D2170" s="160"/>
-      <c r="E2170" s="160"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24218,26 +24220,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24250,111 +24337,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24381,51 +24383,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="188" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="185"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="182" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="182"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="184"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -24642,19 +24644,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="180" t="s">
+      <c r="A20" s="182" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="183"/>
+      <c r="E20" s="183"/>
+      <c r="F20" s="183"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+      <c r="K20" s="184"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -24871,19 +24873,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
+      <c r="B37" s="183"/>
+      <c r="C37" s="183"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="183"/>
+      <c r="F37" s="183"/>
+      <c r="G37" s="183"/>
+      <c r="H37" s="183"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="183"/>
+      <c r="K37" s="184"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25141,28 +25143,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="187"/>
+      <c r="A3" s="189"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="188"/>
+      <c r="A4" s="190"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="188"/>
+      <c r="A5" s="190"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="188"/>
+      <c r="A6" s="190"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="188"/>
+      <c r="A7" s="190"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="188"/>
+      <c r="A8" s="190"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="188"/>
+      <c r="A9" s="190"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="189"/>
+      <c r="A10" s="191"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25345,10 +25347,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="191"/>
+      <c r="C1" s="193"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25359,7 +25361,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="194" t="s">
         <v>209</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25373,7 +25375,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="193"/>
+      <c r="A4" s="195"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25385,7 +25387,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="193"/>
+      <c r="A5" s="195"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25394,7 +25396,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="193"/>
+      <c r="A6" s="195"/>
       <c r="B6" s="139" t="s">
         <v>211</v>
       </c>
@@ -25406,7 +25408,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="193"/>
+      <c r="A7" s="195"/>
       <c r="B7" s="128" t="s">
         <v>177</v>
       </c>
@@ -25418,7 +25420,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="193"/>
+      <c r="A8" s="195"/>
       <c r="B8" s="128" t="s">
         <v>178</v>
       </c>
@@ -25427,7 +25429,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="196"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25442,7 +25444,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="194" t="s">
         <v>210</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25456,7 +25458,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="193"/>
+      <c r="A12" s="195"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25468,7 +25470,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="193"/>
+      <c r="A13" s="195"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25477,7 +25479,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="193"/>
+      <c r="A14" s="195"/>
       <c r="B14" s="139" t="s">
         <v>211</v>
       </c>
@@ -25489,7 +25491,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="193"/>
+      <c r="A15" s="195"/>
       <c r="B15" s="128" t="s">
         <v>177</v>
       </c>
@@ -25501,7 +25503,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="193"/>
+      <c r="A16" s="195"/>
       <c r="B16" s="128" t="s">
         <v>178</v>
       </c>
@@ -25510,7 +25512,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="194"/>
+      <c r="A17" s="196"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25525,7 +25527,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="192" t="s">
+      <c r="A19" s="194" t="s">
         <v>210</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25534,7 +25536,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="193"/>
+      <c r="A20" s="195"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25544,14 +25546,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="195"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="193"/>
+      <c r="A22" s="195"/>
       <c r="B22" s="139" t="s">
         <v>211</v>
       </c>
@@ -25561,7 +25563,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="193"/>
+      <c r="A23" s="195"/>
       <c r="B23" s="128" t="s">
         <v>177</v>
       </c>
@@ -25571,14 +25573,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="193"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="128" t="s">
         <v>178</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="194"/>
+      <c r="A25" s="196"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25613,163 +25615,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="205"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="202"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="215" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="202"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="208"/>
-      <c r="B4" s="209"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="206" t="s">
+      <c r="A5" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="207"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="212" t="s">
+      <c r="A7" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="213"/>
+      <c r="B7" s="202"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="210" t="s">
+      <c r="A9" s="203" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="211"/>
+      <c r="B9" s="204"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="197"/>
-      <c r="B10" s="198"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="206"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="197" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="200"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="199" t="s">
+      <c r="A12" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="200"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="199" t="s">
+      <c r="A13" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="200"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="199" t="s">
+      <c r="A14" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="200"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="199" t="s">
+      <c r="A15" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="200"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="199" t="s">
+      <c r="A16" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="200"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="196"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="212" t="s">
+      <c r="A19" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="213"/>
+      <c r="B19" s="202"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="210" t="s">
+      <c r="A21" s="203" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="211"/>
+      <c r="B21" s="204"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="197"/>
-      <c r="B22" s="198"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="206"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="199" t="s">
+      <c r="A23" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="200"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="199"/>
-      <c r="B24" s="200"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="199" t="s">
+      <c r="A25" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="200"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="199" t="s">
+      <c r="A26" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="200"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25780,6 +25769,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Saved about 46 more frames and updated frame counts.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,7 +14,7 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2025,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2083,34 +2083,20 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2120,6 +2106,20 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,8 +2430,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2838,13 +2838,15 @@
       <c r="B24" s="150" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="101"/>
+      <c r="C24" s="101">
+        <v>1954</v>
+      </c>
       <c r="D24" s="101">
         <v>1969</v>
       </c>
       <c r="E24" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F24" s="105"/>
     </row>
@@ -2854,14 +2856,14 @@
         <v>226</v>
       </c>
       <c r="C25" s="101">
-        <v>2181</v>
+        <v>2179</v>
       </c>
       <c r="D25" s="101">
         <v>2227</v>
       </c>
       <c r="E25" s="123">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F25" s="105"/>
     </row>
@@ -2870,13 +2872,15 @@
       <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
-      <c r="C26" s="101"/>
+      <c r="C26" s="101">
+        <v>2602</v>
+      </c>
       <c r="D26" s="101">
         <v>2696</v>
       </c>
       <c r="E26" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="F26" s="105"/>
     </row>
@@ -4486,11 +4490,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4499,6 +4498,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4530,13 +4534,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4566,18 +4570,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4729,9 +4733,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4882,9 +4886,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="161"/>
+      <c r="D38" s="162"/>
+      <c r="E38" s="162"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5035,9 +5039,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="161"/>
+      <c r="D55" s="162"/>
+      <c r="E55" s="162"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5188,9 +5192,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="161"/>
+      <c r="D72" s="162"/>
+      <c r="E72" s="162"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5341,9 +5345,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="161"/>
+      <c r="D89" s="162"/>
+      <c r="E89" s="162"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5494,9 +5498,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="161"/>
+      <c r="D106" s="162"/>
+      <c r="E106" s="162"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5647,9 +5651,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="161"/>
+      <c r="D123" s="162"/>
+      <c r="E123" s="162"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5800,9 +5804,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="161"/>
+      <c r="D140" s="162"/>
+      <c r="E140" s="162"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5953,9 +5957,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="161"/>
+      <c r="D157" s="162"/>
+      <c r="E157" s="162"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6106,9 +6110,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="161"/>
+      <c r="D174" s="162"/>
+      <c r="E174" s="162"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6259,9 +6263,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="161"/>
+      <c r="D191" s="162"/>
+      <c r="E191" s="162"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6412,9 +6416,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="161"/>
+      <c r="D208" s="162"/>
+      <c r="E208" s="162"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6565,9 +6569,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="161"/>
+      <c r="D225" s="162"/>
+      <c r="E225" s="162"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6718,9 +6722,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="161"/>
+      <c r="D242" s="162"/>
+      <c r="E242" s="162"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6871,9 +6875,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="161"/>
+      <c r="D259" s="162"/>
+      <c r="E259" s="162"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7024,18 +7028,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="168"/>
-      <c r="D276" s="169"/>
-      <c r="E276" s="169"/>
+      <c r="C276" s="177"/>
+      <c r="D276" s="178"/>
+      <c r="E276" s="178"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="161"/>
+      <c r="D277" s="162"/>
+      <c r="E277" s="162"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7186,9 +7190,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="163"/>
+      <c r="D294" s="164"/>
+      <c r="E294" s="164"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7339,9 +7343,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="161"/>
+      <c r="D311" s="162"/>
+      <c r="E311" s="162"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7492,9 +7496,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="161"/>
+      <c r="D328" s="162"/>
+      <c r="E328" s="162"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7645,9 +7649,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="161"/>
+      <c r="D345" s="162"/>
+      <c r="E345" s="162"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7798,9 +7802,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="161"/>
+      <c r="D362" s="162"/>
+      <c r="E362" s="162"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7951,9 +7955,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="161"/>
+      <c r="D379" s="162"/>
+      <c r="E379" s="162"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8104,9 +8108,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="161"/>
+      <c r="D396" s="162"/>
+      <c r="E396" s="162"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8257,9 +8261,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="161"/>
+      <c r="D413" s="162"/>
+      <c r="E413" s="162"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8410,9 +8414,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="161"/>
+      <c r="D430" s="162"/>
+      <c r="E430" s="162"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8563,9 +8567,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="161"/>
+      <c r="D447" s="162"/>
+      <c r="E447" s="162"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8716,9 +8720,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="161"/>
+      <c r="D464" s="162"/>
+      <c r="E464" s="162"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8869,9 +8873,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="161"/>
+      <c r="D481" s="162"/>
+      <c r="E481" s="162"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9022,9 +9026,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="161"/>
+      <c r="D498" s="162"/>
+      <c r="E498" s="162"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9175,9 +9179,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="161"/>
+      <c r="D515" s="162"/>
+      <c r="E515" s="162"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9328,9 +9332,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="161"/>
+      <c r="D532" s="162"/>
+      <c r="E532" s="162"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9481,18 +9485,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="170"/>
-      <c r="D549" s="171"/>
-      <c r="E549" s="171"/>
+      <c r="C549" s="175"/>
+      <c r="D549" s="176"/>
+      <c r="E549" s="176"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="161"/>
+      <c r="D550" s="162"/>
+      <c r="E550" s="162"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9643,9 +9647,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="163"/>
+      <c r="D567" s="164"/>
+      <c r="E567" s="164"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9796,9 +9800,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="161"/>
+      <c r="D584" s="162"/>
+      <c r="E584" s="162"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9949,9 +9953,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="161"/>
+      <c r="D601" s="162"/>
+      <c r="E601" s="162"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10102,9 +10106,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="161"/>
+      <c r="D618" s="162"/>
+      <c r="E618" s="162"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10255,9 +10259,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="161"/>
+      <c r="D635" s="162"/>
+      <c r="E635" s="162"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10408,9 +10412,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="161"/>
+      <c r="D652" s="162"/>
+      <c r="E652" s="162"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10561,9 +10565,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="161"/>
+      <c r="D669" s="162"/>
+      <c r="E669" s="162"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10714,9 +10718,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="161"/>
+      <c r="D686" s="162"/>
+      <c r="E686" s="162"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10867,9 +10871,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="161"/>
+      <c r="D703" s="162"/>
+      <c r="E703" s="162"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11020,9 +11024,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="161"/>
+      <c r="D720" s="162"/>
+      <c r="E720" s="162"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11173,9 +11177,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="161"/>
+      <c r="D737" s="162"/>
+      <c r="E737" s="162"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11326,9 +11330,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="161"/>
+      <c r="D754" s="162"/>
+      <c r="E754" s="162"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11479,9 +11483,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="161"/>
+      <c r="D771" s="162"/>
+      <c r="E771" s="162"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11632,9 +11636,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="161"/>
+      <c r="D788" s="162"/>
+      <c r="E788" s="162"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11785,9 +11789,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="161"/>
+      <c r="D805" s="162"/>
+      <c r="E805" s="162"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11938,18 +11942,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="172"/>
-      <c r="D822" s="173"/>
-      <c r="E822" s="173"/>
+      <c r="C822" s="173"/>
+      <c r="D822" s="174"/>
+      <c r="E822" s="174"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="161"/>
+      <c r="D823" s="162"/>
+      <c r="E823" s="162"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12100,9 +12104,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="163"/>
+      <c r="D840" s="164"/>
+      <c r="E840" s="164"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12253,9 +12257,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="161"/>
+      <c r="D857" s="162"/>
+      <c r="E857" s="162"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12406,9 +12410,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="161"/>
+      <c r="D874" s="162"/>
+      <c r="E874" s="162"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12559,9 +12563,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="161"/>
+      <c r="D891" s="162"/>
+      <c r="E891" s="162"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12712,9 +12716,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="161"/>
+      <c r="D908" s="162"/>
+      <c r="E908" s="162"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12865,9 +12869,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="161"/>
+      <c r="D925" s="162"/>
+      <c r="E925" s="162"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13018,9 +13022,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="161"/>
+      <c r="D942" s="162"/>
+      <c r="E942" s="162"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13171,9 +13175,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="161"/>
+      <c r="D959" s="162"/>
+      <c r="E959" s="162"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13324,9 +13328,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="161"/>
+      <c r="D976" s="162"/>
+      <c r="E976" s="162"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13477,9 +13481,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="161"/>
+      <c r="D993" s="162"/>
+      <c r="E993" s="162"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13630,9 +13634,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="161"/>
+      <c r="D1010" s="162"/>
+      <c r="E1010" s="162"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13783,9 +13787,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="161"/>
+      <c r="D1027" s="162"/>
+      <c r="E1027" s="162"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13936,9 +13940,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="161"/>
+      <c r="D1044" s="162"/>
+      <c r="E1044" s="162"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14089,9 +14093,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="161"/>
+      <c r="D1061" s="162"/>
+      <c r="E1061" s="162"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14242,9 +14246,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="161"/>
+      <c r="D1078" s="162"/>
+      <c r="E1078" s="162"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14395,18 +14399,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="171"/>
+      <c r="D1095" s="172"/>
+      <c r="E1095" s="172"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="161"/>
+      <c r="D1096" s="162"/>
+      <c r="E1096" s="162"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14557,9 +14561,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="163"/>
+      <c r="D1113" s="164"/>
+      <c r="E1113" s="164"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14710,9 +14714,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="161"/>
+      <c r="D1130" s="162"/>
+      <c r="E1130" s="162"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14863,9 +14867,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="161"/>
+      <c r="D1147" s="162"/>
+      <c r="E1147" s="162"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15016,9 +15020,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="161"/>
+      <c r="D1164" s="162"/>
+      <c r="E1164" s="162"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15169,9 +15173,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="161"/>
+      <c r="D1181" s="162"/>
+      <c r="E1181" s="162"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15322,9 +15326,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="161"/>
+      <c r="D1198" s="162"/>
+      <c r="E1198" s="162"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15475,9 +15479,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="161"/>
+      <c r="D1215" s="162"/>
+      <c r="E1215" s="162"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15628,9 +15632,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="161"/>
+      <c r="D1232" s="162"/>
+      <c r="E1232" s="162"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15781,9 +15785,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="161"/>
+      <c r="D1249" s="162"/>
+      <c r="E1249" s="162"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15934,9 +15938,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="161"/>
+      <c r="D1266" s="162"/>
+      <c r="E1266" s="162"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16087,9 +16091,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="161"/>
+      <c r="D1283" s="162"/>
+      <c r="E1283" s="162"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16240,9 +16244,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="161"/>
+      <c r="D1300" s="162"/>
+      <c r="E1300" s="162"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16393,9 +16397,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="161"/>
+      <c r="D1317" s="162"/>
+      <c r="E1317" s="162"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16546,9 +16550,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="161"/>
+      <c r="D1334" s="162"/>
+      <c r="E1334" s="162"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16699,9 +16703,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="161"/>
+      <c r="D1351" s="162"/>
+      <c r="E1351" s="162"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16852,18 +16856,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="176"/>
-      <c r="D1368" s="177"/>
-      <c r="E1368" s="177"/>
+      <c r="C1368" s="169"/>
+      <c r="D1368" s="170"/>
+      <c r="E1368" s="170"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="161"/>
+      <c r="D1369" s="162"/>
+      <c r="E1369" s="162"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17014,9 +17018,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="163"/>
+      <c r="D1386" s="164"/>
+      <c r="E1386" s="164"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17167,9 +17171,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="161"/>
+      <c r="D1403" s="162"/>
+      <c r="E1403" s="162"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17320,9 +17324,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="161"/>
+      <c r="D1420" s="162"/>
+      <c r="E1420" s="162"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17473,9 +17477,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="161"/>
+      <c r="D1437" s="162"/>
+      <c r="E1437" s="162"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17626,9 +17630,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="161"/>
+      <c r="D1454" s="162"/>
+      <c r="E1454" s="162"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17779,9 +17783,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="161"/>
+      <c r="D1471" s="162"/>
+      <c r="E1471" s="162"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17932,9 +17936,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="161"/>
+      <c r="D1488" s="162"/>
+      <c r="E1488" s="162"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18085,9 +18089,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="161"/>
+      <c r="D1505" s="162"/>
+      <c r="E1505" s="162"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18238,9 +18242,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="161"/>
+      <c r="D1522" s="162"/>
+      <c r="E1522" s="162"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18391,9 +18395,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="161"/>
+      <c r="D1539" s="162"/>
+      <c r="E1539" s="162"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18544,9 +18548,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="161"/>
+      <c r="D1556" s="162"/>
+      <c r="E1556" s="162"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18697,9 +18701,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="161"/>
+      <c r="D1573" s="162"/>
+      <c r="E1573" s="162"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18850,9 +18854,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="161"/>
+      <c r="D1590" s="162"/>
+      <c r="E1590" s="162"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19003,9 +19007,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="161"/>
+      <c r="D1607" s="162"/>
+      <c r="E1607" s="162"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19156,9 +19160,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="161"/>
+      <c r="D1624" s="162"/>
+      <c r="E1624" s="162"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19309,18 +19313,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="178"/>
-      <c r="D1641" s="179"/>
-      <c r="E1641" s="179"/>
+      <c r="C1641" s="167"/>
+      <c r="D1641" s="168"/>
+      <c r="E1641" s="168"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="161"/>
+      <c r="D1642" s="162"/>
+      <c r="E1642" s="162"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19471,9 +19475,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="163"/>
+      <c r="D1659" s="164"/>
+      <c r="E1659" s="164"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19624,9 +19628,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="161"/>
+      <c r="D1676" s="162"/>
+      <c r="E1676" s="162"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19777,9 +19781,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="161"/>
+      <c r="D1693" s="162"/>
+      <c r="E1693" s="162"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19930,9 +19934,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="161"/>
+      <c r="D1710" s="162"/>
+      <c r="E1710" s="162"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20083,9 +20087,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="161"/>
+      <c r="D1727" s="162"/>
+      <c r="E1727" s="162"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20236,9 +20240,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="161"/>
+      <c r="D1744" s="162"/>
+      <c r="E1744" s="162"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20389,9 +20393,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="161"/>
+      <c r="D1761" s="162"/>
+      <c r="E1761" s="162"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20542,9 +20546,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="161"/>
+      <c r="D1778" s="162"/>
+      <c r="E1778" s="162"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20695,9 +20699,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="161"/>
+      <c r="D1795" s="162"/>
+      <c r="E1795" s="162"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20848,9 +20852,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="161"/>
+      <c r="D1812" s="162"/>
+      <c r="E1812" s="162"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21001,9 +21005,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="161"/>
+      <c r="D1829" s="162"/>
+      <c r="E1829" s="162"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21154,9 +21158,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="161"/>
+      <c r="D1846" s="162"/>
+      <c r="E1846" s="162"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21307,9 +21311,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="161"/>
+      <c r="D1863" s="162"/>
+      <c r="E1863" s="162"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21460,9 +21464,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="161"/>
+      <c r="D1880" s="162"/>
+      <c r="E1880" s="162"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21613,9 +21617,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="161"/>
+      <c r="D1897" s="162"/>
+      <c r="E1897" s="162"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21766,18 +21770,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="180"/>
-      <c r="D1914" s="181"/>
-      <c r="E1914" s="181"/>
+      <c r="C1914" s="165"/>
+      <c r="D1914" s="166"/>
+      <c r="E1914" s="166"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="161"/>
+      <c r="D1915" s="162"/>
+      <c r="E1915" s="162"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21928,9 +21932,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="163"/>
+      <c r="D1932" s="164"/>
+      <c r="E1932" s="164"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22081,9 +22085,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="161"/>
+      <c r="D1949" s="162"/>
+      <c r="E1949" s="162"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22234,9 +22238,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="161"/>
+      <c r="D1966" s="162"/>
+      <c r="E1966" s="162"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22387,9 +22391,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="161"/>
+      <c r="D1983" s="162"/>
+      <c r="E1983" s="162"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22540,9 +22544,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="161"/>
+      <c r="D2000" s="162"/>
+      <c r="E2000" s="162"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22693,9 +22697,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="161"/>
+      <c r="D2017" s="162"/>
+      <c r="E2017" s="162"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22846,9 +22850,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="161"/>
+      <c r="D2034" s="162"/>
+      <c r="E2034" s="162"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22999,9 +23003,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="161"/>
+      <c r="D2051" s="162"/>
+      <c r="E2051" s="162"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23152,9 +23156,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="161"/>
+      <c r="D2068" s="162"/>
+      <c r="E2068" s="162"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23305,9 +23309,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="161"/>
+      <c r="D2085" s="162"/>
+      <c r="E2085" s="162"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23458,9 +23462,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="161"/>
+      <c r="D2102" s="162"/>
+      <c r="E2102" s="162"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23611,9 +23615,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="161"/>
+      <c r="D2119" s="162"/>
+      <c r="E2119" s="162"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23764,9 +23768,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="161"/>
+      <c r="D2136" s="162"/>
+      <c r="E2136" s="162"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23917,9 +23921,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="161"/>
+      <c r="D2153" s="162"/>
+      <c r="E2153" s="162"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24070,9 +24074,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="161"/>
+      <c r="D2170" s="162"/>
+      <c r="E2170" s="162"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24220,15 +24224,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24241,122 +24352,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25615,150 +25619,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="206" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="208"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="203" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="214"/>
+      <c r="B2" s="204"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="214"/>
+      <c r="B3" s="204"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="211"/>
-      <c r="B4" s="212"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="209" t="s">
+      <c r="A5" s="208" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="210"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="201" t="s">
+      <c r="A7" s="214" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="202"/>
+      <c r="B7" s="215"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="204"/>
+      <c r="B9" s="213"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="205"/>
-      <c r="B10" s="206"/>
+      <c r="A10" s="199"/>
+      <c r="B10" s="200"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="198"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="197" t="s">
+      <c r="A12" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="198"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="198"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="198"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="197" t="s">
+      <c r="A15" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="198"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="197" t="s">
+      <c r="A16" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="198"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="200"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="214" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="202"/>
+      <c r="B19" s="215"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="203" t="s">
+      <c r="A21" s="212" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="204"/>
+      <c r="B21" s="213"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="205"/>
-      <c r="B22" s="206"/>
+      <c r="A22" s="199"/>
+      <c r="B22" s="200"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="197" t="s">
+      <c r="A23" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="198"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="197"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="197" t="s">
+      <c r="A25" s="201" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="198"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="197" t="s">
+      <c r="A26" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="198"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25769,19 +25786,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Saved an additional 28 frames from going to hostage #3.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -2025,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2083,20 +2083,34 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2106,20 +2120,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,7 +2430,7 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -4490,6 +4490,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4498,11 +4503,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4534,13 +4534,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4570,18 +4570,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4733,9 +4733,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4886,9 +4886,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5039,9 +5039,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="161"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5192,9 +5192,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="161"/>
-      <c r="D72" s="162"/>
-      <c r="E72" s="162"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5345,9 +5345,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="161"/>
-      <c r="D89" s="162"/>
-      <c r="E89" s="162"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5498,9 +5498,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="161"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5651,9 +5651,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="162"/>
-      <c r="E123" s="162"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5804,9 +5804,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="161"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="162"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5957,9 +5957,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="162"/>
-      <c r="E157" s="162"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6110,9 +6110,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="162"/>
-      <c r="E174" s="162"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6263,9 +6263,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="162"/>
-      <c r="E191" s="162"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6416,9 +6416,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="162"/>
-      <c r="E208" s="162"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6569,9 +6569,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="162"/>
-      <c r="E225" s="162"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6722,9 +6722,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="161"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6875,9 +6875,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="161"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7028,18 +7028,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="177"/>
-      <c r="D276" s="178"/>
-      <c r="E276" s="178"/>
+      <c r="C276" s="168"/>
+      <c r="D276" s="169"/>
+      <c r="E276" s="169"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="161"/>
-      <c r="D277" s="162"/>
-      <c r="E277" s="162"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7190,9 +7190,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="163"/>
-      <c r="D294" s="164"/>
-      <c r="E294" s="164"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7343,9 +7343,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="161"/>
-      <c r="D311" s="162"/>
-      <c r="E311" s="162"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7496,9 +7496,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="161"/>
-      <c r="D328" s="162"/>
-      <c r="E328" s="162"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7649,9 +7649,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="161"/>
-      <c r="D345" s="162"/>
-      <c r="E345" s="162"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7802,9 +7802,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="161"/>
-      <c r="D362" s="162"/>
-      <c r="E362" s="162"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7955,9 +7955,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="161"/>
-      <c r="D379" s="162"/>
-      <c r="E379" s="162"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8108,9 +8108,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="161"/>
-      <c r="D396" s="162"/>
-      <c r="E396" s="162"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8261,9 +8261,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="161"/>
-      <c r="D413" s="162"/>
-      <c r="E413" s="162"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8414,9 +8414,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="161"/>
-      <c r="D430" s="162"/>
-      <c r="E430" s="162"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8567,9 +8567,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="161"/>
-      <c r="D447" s="162"/>
-      <c r="E447" s="162"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8720,9 +8720,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="161"/>
-      <c r="D464" s="162"/>
-      <c r="E464" s="162"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8873,9 +8873,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="161"/>
-      <c r="D481" s="162"/>
-      <c r="E481" s="162"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9026,9 +9026,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="161"/>
-      <c r="D498" s="162"/>
-      <c r="E498" s="162"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9179,9 +9179,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="161"/>
-      <c r="D515" s="162"/>
-      <c r="E515" s="162"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9332,9 +9332,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="161"/>
-      <c r="D532" s="162"/>
-      <c r="E532" s="162"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9485,18 +9485,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="170"/>
+      <c r="D549" s="171"/>
+      <c r="E549" s="171"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="161"/>
-      <c r="D550" s="162"/>
-      <c r="E550" s="162"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9647,9 +9647,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="163"/>
-      <c r="D567" s="164"/>
-      <c r="E567" s="164"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9800,9 +9800,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="161"/>
-      <c r="D584" s="162"/>
-      <c r="E584" s="162"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9953,9 +9953,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="161"/>
-      <c r="D601" s="162"/>
-      <c r="E601" s="162"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10106,9 +10106,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="161"/>
-      <c r="D618" s="162"/>
-      <c r="E618" s="162"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10259,9 +10259,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="161"/>
-      <c r="D635" s="162"/>
-      <c r="E635" s="162"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10412,9 +10412,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="161"/>
-      <c r="D652" s="162"/>
-      <c r="E652" s="162"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10565,9 +10565,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="161"/>
-      <c r="D669" s="162"/>
-      <c r="E669" s="162"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10718,9 +10718,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="161"/>
-      <c r="D686" s="162"/>
-      <c r="E686" s="162"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10871,9 +10871,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="161"/>
-      <c r="D703" s="162"/>
-      <c r="E703" s="162"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11024,9 +11024,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="161"/>
-      <c r="D720" s="162"/>
-      <c r="E720" s="162"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11177,9 +11177,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="161"/>
-      <c r="D737" s="162"/>
-      <c r="E737" s="162"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11330,9 +11330,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="161"/>
-      <c r="D754" s="162"/>
-      <c r="E754" s="162"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11483,9 +11483,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="161"/>
-      <c r="D771" s="162"/>
-      <c r="E771" s="162"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11636,9 +11636,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="161"/>
-      <c r="D788" s="162"/>
-      <c r="E788" s="162"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11789,9 +11789,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="161"/>
-      <c r="D805" s="162"/>
-      <c r="E805" s="162"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11942,18 +11942,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="173"/>
-      <c r="D822" s="174"/>
-      <c r="E822" s="174"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="161"/>
-      <c r="D823" s="162"/>
-      <c r="E823" s="162"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12104,9 +12104,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="163"/>
-      <c r="D840" s="164"/>
-      <c r="E840" s="164"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12257,9 +12257,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="161"/>
-      <c r="D857" s="162"/>
-      <c r="E857" s="162"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12410,9 +12410,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="161"/>
-      <c r="D874" s="162"/>
-      <c r="E874" s="162"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12563,9 +12563,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="161"/>
-      <c r="D891" s="162"/>
-      <c r="E891" s="162"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12716,9 +12716,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="161"/>
-      <c r="D908" s="162"/>
-      <c r="E908" s="162"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12869,9 +12869,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="161"/>
-      <c r="D925" s="162"/>
-      <c r="E925" s="162"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13022,9 +13022,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="161"/>
-      <c r="D942" s="162"/>
-      <c r="E942" s="162"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13175,9 +13175,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="161"/>
-      <c r="D959" s="162"/>
-      <c r="E959" s="162"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13328,9 +13328,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="161"/>
-      <c r="D976" s="162"/>
-      <c r="E976" s="162"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13481,9 +13481,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="161"/>
-      <c r="D993" s="162"/>
-      <c r="E993" s="162"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13634,9 +13634,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="161"/>
-      <c r="D1010" s="162"/>
-      <c r="E1010" s="162"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13787,9 +13787,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="161"/>
-      <c r="D1027" s="162"/>
-      <c r="E1027" s="162"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13940,9 +13940,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="161"/>
-      <c r="D1044" s="162"/>
-      <c r="E1044" s="162"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14093,9 +14093,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="161"/>
-      <c r="D1061" s="162"/>
-      <c r="E1061" s="162"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14246,9 +14246,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="161"/>
-      <c r="D1078" s="162"/>
-      <c r="E1078" s="162"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14399,18 +14399,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="171"/>
-      <c r="D1095" s="172"/>
-      <c r="E1095" s="172"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="161"/>
-      <c r="D1096" s="162"/>
-      <c r="E1096" s="162"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14561,9 +14561,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="163"/>
-      <c r="D1113" s="164"/>
-      <c r="E1113" s="164"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14714,9 +14714,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="161"/>
-      <c r="D1130" s="162"/>
-      <c r="E1130" s="162"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14867,9 +14867,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="161"/>
-      <c r="D1147" s="162"/>
-      <c r="E1147" s="162"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15020,9 +15020,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="161"/>
-      <c r="D1164" s="162"/>
-      <c r="E1164" s="162"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15173,9 +15173,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="161"/>
-      <c r="D1181" s="162"/>
-      <c r="E1181" s="162"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15326,9 +15326,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="161"/>
-      <c r="D1198" s="162"/>
-      <c r="E1198" s="162"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15479,9 +15479,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="161"/>
-      <c r="D1215" s="162"/>
-      <c r="E1215" s="162"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15632,9 +15632,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="161"/>
-      <c r="D1232" s="162"/>
-      <c r="E1232" s="162"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15785,9 +15785,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="161"/>
-      <c r="D1249" s="162"/>
-      <c r="E1249" s="162"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15938,9 +15938,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="161"/>
-      <c r="D1266" s="162"/>
-      <c r="E1266" s="162"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16091,9 +16091,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="161"/>
-      <c r="D1283" s="162"/>
-      <c r="E1283" s="162"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16244,9 +16244,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="161"/>
-      <c r="D1300" s="162"/>
-      <c r="E1300" s="162"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16397,9 +16397,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="161"/>
-      <c r="D1317" s="162"/>
-      <c r="E1317" s="162"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16550,9 +16550,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="161"/>
-      <c r="D1334" s="162"/>
-      <c r="E1334" s="162"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16703,9 +16703,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="161"/>
-      <c r="D1351" s="162"/>
-      <c r="E1351" s="162"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16856,18 +16856,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="169"/>
-      <c r="D1368" s="170"/>
-      <c r="E1368" s="170"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="161"/>
-      <c r="D1369" s="162"/>
-      <c r="E1369" s="162"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17018,9 +17018,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="163"/>
-      <c r="D1386" s="164"/>
-      <c r="E1386" s="164"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17171,9 +17171,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="161"/>
-      <c r="D1403" s="162"/>
-      <c r="E1403" s="162"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17324,9 +17324,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="161"/>
-      <c r="D1420" s="162"/>
-      <c r="E1420" s="162"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17477,9 +17477,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="161"/>
-      <c r="D1437" s="162"/>
-      <c r="E1437" s="162"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17630,9 +17630,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="161"/>
-      <c r="D1454" s="162"/>
-      <c r="E1454" s="162"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17783,9 +17783,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="161"/>
-      <c r="D1471" s="162"/>
-      <c r="E1471" s="162"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17936,9 +17936,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="161"/>
-      <c r="D1488" s="162"/>
-      <c r="E1488" s="162"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18089,9 +18089,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="161"/>
-      <c r="D1505" s="162"/>
-      <c r="E1505" s="162"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18242,9 +18242,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="161"/>
-      <c r="D1522" s="162"/>
-      <c r="E1522" s="162"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18395,9 +18395,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="161"/>
-      <c r="D1539" s="162"/>
-      <c r="E1539" s="162"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18548,9 +18548,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="161"/>
-      <c r="D1556" s="162"/>
-      <c r="E1556" s="162"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18701,9 +18701,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="161"/>
-      <c r="D1573" s="162"/>
-      <c r="E1573" s="162"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18854,9 +18854,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="161"/>
-      <c r="D1590" s="162"/>
-      <c r="E1590" s="162"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19007,9 +19007,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="161"/>
-      <c r="D1607" s="162"/>
-      <c r="E1607" s="162"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19160,9 +19160,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="161"/>
-      <c r="D1624" s="162"/>
-      <c r="E1624" s="162"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19313,18 +19313,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="167"/>
-      <c r="D1641" s="168"/>
-      <c r="E1641" s="168"/>
+      <c r="C1641" s="178"/>
+      <c r="D1641" s="179"/>
+      <c r="E1641" s="179"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="161"/>
-      <c r="D1642" s="162"/>
-      <c r="E1642" s="162"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19475,9 +19475,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="163"/>
-      <c r="D1659" s="164"/>
-      <c r="E1659" s="164"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19628,9 +19628,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="161"/>
-      <c r="D1676" s="162"/>
-      <c r="E1676" s="162"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19781,9 +19781,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="161"/>
-      <c r="D1693" s="162"/>
-      <c r="E1693" s="162"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19934,9 +19934,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="161"/>
-      <c r="D1710" s="162"/>
-      <c r="E1710" s="162"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20087,9 +20087,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="161"/>
-      <c r="D1727" s="162"/>
-      <c r="E1727" s="162"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20240,9 +20240,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="161"/>
-      <c r="D1744" s="162"/>
-      <c r="E1744" s="162"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20393,9 +20393,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="161"/>
-      <c r="D1761" s="162"/>
-      <c r="E1761" s="162"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20546,9 +20546,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="161"/>
-      <c r="D1778" s="162"/>
-      <c r="E1778" s="162"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20699,9 +20699,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="161"/>
-      <c r="D1795" s="162"/>
-      <c r="E1795" s="162"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20852,9 +20852,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="161"/>
-      <c r="D1812" s="162"/>
-      <c r="E1812" s="162"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21005,9 +21005,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="161"/>
-      <c r="D1829" s="162"/>
-      <c r="E1829" s="162"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21158,9 +21158,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="161"/>
-      <c r="D1846" s="162"/>
-      <c r="E1846" s="162"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21311,9 +21311,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="161"/>
-      <c r="D1863" s="162"/>
-      <c r="E1863" s="162"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21464,9 +21464,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="161"/>
-      <c r="D1880" s="162"/>
-      <c r="E1880" s="162"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21617,9 +21617,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="161"/>
-      <c r="D1897" s="162"/>
-      <c r="E1897" s="162"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21770,18 +21770,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="165"/>
-      <c r="D1914" s="166"/>
-      <c r="E1914" s="166"/>
+      <c r="C1914" s="180"/>
+      <c r="D1914" s="181"/>
+      <c r="E1914" s="181"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="161"/>
-      <c r="D1915" s="162"/>
-      <c r="E1915" s="162"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21932,9 +21932,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="163"/>
-      <c r="D1932" s="164"/>
-      <c r="E1932" s="164"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22085,9 +22085,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="161"/>
-      <c r="D1949" s="162"/>
-      <c r="E1949" s="162"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22238,9 +22238,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="161"/>
-      <c r="D1966" s="162"/>
-      <c r="E1966" s="162"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22391,9 +22391,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="161"/>
-      <c r="D1983" s="162"/>
-      <c r="E1983" s="162"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22544,9 +22544,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="161"/>
-      <c r="D2000" s="162"/>
-      <c r="E2000" s="162"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22697,9 +22697,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="161"/>
-      <c r="D2017" s="162"/>
-      <c r="E2017" s="162"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22850,9 +22850,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="161"/>
-      <c r="D2034" s="162"/>
-      <c r="E2034" s="162"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23003,9 +23003,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="161"/>
-      <c r="D2051" s="162"/>
-      <c r="E2051" s="162"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23156,9 +23156,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="161"/>
-      <c r="D2068" s="162"/>
-      <c r="E2068" s="162"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23309,9 +23309,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="161"/>
-      <c r="D2085" s="162"/>
-      <c r="E2085" s="162"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23462,9 +23462,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="161"/>
-      <c r="D2102" s="162"/>
-      <c r="E2102" s="162"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23615,9 +23615,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="161"/>
-      <c r="D2119" s="162"/>
-      <c r="E2119" s="162"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23768,9 +23768,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="161"/>
-      <c r="D2136" s="162"/>
-      <c r="E2136" s="162"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23921,9 +23921,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="161"/>
-      <c r="D2153" s="162"/>
-      <c r="E2153" s="162"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24074,9 +24074,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="161"/>
-      <c r="D2170" s="162"/>
-      <c r="E2170" s="162"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24224,26 +24224,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24256,111 +24341,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25340,7 +25340,7 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -25619,163 +25619,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="207"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="215" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="204"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="210"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="208" t="s">
+      <c r="A5" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="209"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="214" t="s">
+      <c r="A7" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="215"/>
+      <c r="B7" s="202"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="203" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="213"/>
+      <c r="B9" s="204"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="206"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="197" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="214" t="s">
+      <c r="A19" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="215"/>
+      <c r="B19" s="202"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="203" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="213"/>
+      <c r="B21" s="204"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="199"/>
-      <c r="B22" s="200"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="206"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25786,6 +25773,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
spiderman2 - avoid damage in a graceful way, and saved 80 frames getting to the 4th hostage.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,7 +14,7 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -2025,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2083,34 +2083,20 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2120,6 +2106,20 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,7 +2430,7 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2889,13 +2889,15 @@
       <c r="B27" s="150" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="101"/>
+      <c r="C27" s="101">
+        <v>2744</v>
+      </c>
       <c r="D27" s="101">
         <v>2866</v>
       </c>
       <c r="E27" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="F27" s="105"/>
     </row>
@@ -2904,13 +2906,15 @@
       <c r="B28" s="150" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="101"/>
+      <c r="C28" s="101">
+        <v>3109</v>
+      </c>
       <c r="D28" s="101">
         <v>3309</v>
       </c>
       <c r="E28" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F28" s="105"/>
     </row>
@@ -4490,11 +4494,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4503,6 +4502,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4534,13 +4538,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4570,18 +4574,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4733,9 +4737,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4886,9 +4890,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="161"/>
+      <c r="D38" s="162"/>
+      <c r="E38" s="162"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5039,9 +5043,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="161"/>
+      <c r="D55" s="162"/>
+      <c r="E55" s="162"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5192,9 +5196,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="161"/>
+      <c r="D72" s="162"/>
+      <c r="E72" s="162"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5345,9 +5349,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="161"/>
+      <c r="D89" s="162"/>
+      <c r="E89" s="162"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5498,9 +5502,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="161"/>
+      <c r="D106" s="162"/>
+      <c r="E106" s="162"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5651,9 +5655,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="161"/>
+      <c r="D123" s="162"/>
+      <c r="E123" s="162"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5804,9 +5808,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="161"/>
+      <c r="D140" s="162"/>
+      <c r="E140" s="162"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5957,9 +5961,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="161"/>
+      <c r="D157" s="162"/>
+      <c r="E157" s="162"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6110,9 +6114,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="161"/>
+      <c r="D174" s="162"/>
+      <c r="E174" s="162"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6263,9 +6267,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="161"/>
+      <c r="D191" s="162"/>
+      <c r="E191" s="162"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6416,9 +6420,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="161"/>
+      <c r="D208" s="162"/>
+      <c r="E208" s="162"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6569,9 +6573,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="161"/>
+      <c r="D225" s="162"/>
+      <c r="E225" s="162"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6722,9 +6726,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="161"/>
+      <c r="D242" s="162"/>
+      <c r="E242" s="162"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6875,9 +6879,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="161"/>
+      <c r="D259" s="162"/>
+      <c r="E259" s="162"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7028,18 +7032,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="168"/>
-      <c r="D276" s="169"/>
-      <c r="E276" s="169"/>
+      <c r="C276" s="177"/>
+      <c r="D276" s="178"/>
+      <c r="E276" s="178"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="161"/>
+      <c r="D277" s="162"/>
+      <c r="E277" s="162"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7190,9 +7194,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="163"/>
+      <c r="D294" s="164"/>
+      <c r="E294" s="164"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7343,9 +7347,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="161"/>
+      <c r="D311" s="162"/>
+      <c r="E311" s="162"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7496,9 +7500,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="161"/>
+      <c r="D328" s="162"/>
+      <c r="E328" s="162"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7649,9 +7653,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="161"/>
+      <c r="D345" s="162"/>
+      <c r="E345" s="162"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7802,9 +7806,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="161"/>
+      <c r="D362" s="162"/>
+      <c r="E362" s="162"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7955,9 +7959,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="161"/>
+      <c r="D379" s="162"/>
+      <c r="E379" s="162"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8108,9 +8112,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="161"/>
+      <c r="D396" s="162"/>
+      <c r="E396" s="162"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8261,9 +8265,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="161"/>
+      <c r="D413" s="162"/>
+      <c r="E413" s="162"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8414,9 +8418,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="161"/>
+      <c r="D430" s="162"/>
+      <c r="E430" s="162"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8567,9 +8571,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="161"/>
+      <c r="D447" s="162"/>
+      <c r="E447" s="162"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8720,9 +8724,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="161"/>
+      <c r="D464" s="162"/>
+      <c r="E464" s="162"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8873,9 +8877,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="161"/>
+      <c r="D481" s="162"/>
+      <c r="E481" s="162"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9026,9 +9030,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="161"/>
+      <c r="D498" s="162"/>
+      <c r="E498" s="162"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9179,9 +9183,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="161"/>
+      <c r="D515" s="162"/>
+      <c r="E515" s="162"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9332,9 +9336,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="161"/>
+      <c r="D532" s="162"/>
+      <c r="E532" s="162"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9485,18 +9489,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="170"/>
-      <c r="D549" s="171"/>
-      <c r="E549" s="171"/>
+      <c r="C549" s="175"/>
+      <c r="D549" s="176"/>
+      <c r="E549" s="176"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="161"/>
+      <c r="D550" s="162"/>
+      <c r="E550" s="162"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9647,9 +9651,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="163"/>
+      <c r="D567" s="164"/>
+      <c r="E567" s="164"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9800,9 +9804,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="161"/>
+      <c r="D584" s="162"/>
+      <c r="E584" s="162"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9953,9 +9957,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="161"/>
+      <c r="D601" s="162"/>
+      <c r="E601" s="162"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10106,9 +10110,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="161"/>
+      <c r="D618" s="162"/>
+      <c r="E618" s="162"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10259,9 +10263,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="161"/>
+      <c r="D635" s="162"/>
+      <c r="E635" s="162"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10412,9 +10416,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="161"/>
+      <c r="D652" s="162"/>
+      <c r="E652" s="162"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10565,9 +10569,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="161"/>
+      <c r="D669" s="162"/>
+      <c r="E669" s="162"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10718,9 +10722,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="161"/>
+      <c r="D686" s="162"/>
+      <c r="E686" s="162"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10871,9 +10875,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="161"/>
+      <c r="D703" s="162"/>
+      <c r="E703" s="162"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11024,9 +11028,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="161"/>
+      <c r="D720" s="162"/>
+      <c r="E720" s="162"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11177,9 +11181,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="161"/>
+      <c r="D737" s="162"/>
+      <c r="E737" s="162"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11330,9 +11334,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="161"/>
+      <c r="D754" s="162"/>
+      <c r="E754" s="162"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11483,9 +11487,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="161"/>
+      <c r="D771" s="162"/>
+      <c r="E771" s="162"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11636,9 +11640,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="161"/>
+      <c r="D788" s="162"/>
+      <c r="E788" s="162"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11789,9 +11793,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="161"/>
+      <c r="D805" s="162"/>
+      <c r="E805" s="162"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11942,18 +11946,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="172"/>
-      <c r="D822" s="173"/>
-      <c r="E822" s="173"/>
+      <c r="C822" s="173"/>
+      <c r="D822" s="174"/>
+      <c r="E822" s="174"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="161"/>
+      <c r="D823" s="162"/>
+      <c r="E823" s="162"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12104,9 +12108,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="163"/>
+      <c r="D840" s="164"/>
+      <c r="E840" s="164"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12257,9 +12261,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="161"/>
+      <c r="D857" s="162"/>
+      <c r="E857" s="162"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12410,9 +12414,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="161"/>
+      <c r="D874" s="162"/>
+      <c r="E874" s="162"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12563,9 +12567,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="161"/>
+      <c r="D891" s="162"/>
+      <c r="E891" s="162"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12716,9 +12720,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="161"/>
+      <c r="D908" s="162"/>
+      <c r="E908" s="162"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12869,9 +12873,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="161"/>
+      <c r="D925" s="162"/>
+      <c r="E925" s="162"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13022,9 +13026,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="161"/>
+      <c r="D942" s="162"/>
+      <c r="E942" s="162"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13175,9 +13179,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="161"/>
+      <c r="D959" s="162"/>
+      <c r="E959" s="162"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13328,9 +13332,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="161"/>
+      <c r="D976" s="162"/>
+      <c r="E976" s="162"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13481,9 +13485,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="161"/>
+      <c r="D993" s="162"/>
+      <c r="E993" s="162"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13634,9 +13638,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="161"/>
+      <c r="D1010" s="162"/>
+      <c r="E1010" s="162"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13787,9 +13791,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="161"/>
+      <c r="D1027" s="162"/>
+      <c r="E1027" s="162"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13940,9 +13944,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="161"/>
+      <c r="D1044" s="162"/>
+      <c r="E1044" s="162"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14093,9 +14097,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="161"/>
+      <c r="D1061" s="162"/>
+      <c r="E1061" s="162"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14246,9 +14250,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="161"/>
+      <c r="D1078" s="162"/>
+      <c r="E1078" s="162"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14399,18 +14403,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="171"/>
+      <c r="D1095" s="172"/>
+      <c r="E1095" s="172"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="161"/>
+      <c r="D1096" s="162"/>
+      <c r="E1096" s="162"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14561,9 +14565,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="163"/>
+      <c r="D1113" s="164"/>
+      <c r="E1113" s="164"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14714,9 +14718,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="161"/>
+      <c r="D1130" s="162"/>
+      <c r="E1130" s="162"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14867,9 +14871,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="161"/>
+      <c r="D1147" s="162"/>
+      <c r="E1147" s="162"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15020,9 +15024,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="161"/>
+      <c r="D1164" s="162"/>
+      <c r="E1164" s="162"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15173,9 +15177,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="161"/>
+      <c r="D1181" s="162"/>
+      <c r="E1181" s="162"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15326,9 +15330,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="161"/>
+      <c r="D1198" s="162"/>
+      <c r="E1198" s="162"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15479,9 +15483,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="161"/>
+      <c r="D1215" s="162"/>
+      <c r="E1215" s="162"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15632,9 +15636,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="161"/>
+      <c r="D1232" s="162"/>
+      <c r="E1232" s="162"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15785,9 +15789,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="161"/>
+      <c r="D1249" s="162"/>
+      <c r="E1249" s="162"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15938,9 +15942,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="161"/>
+      <c r="D1266" s="162"/>
+      <c r="E1266" s="162"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16091,9 +16095,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="161"/>
+      <c r="D1283" s="162"/>
+      <c r="E1283" s="162"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16244,9 +16248,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="161"/>
+      <c r="D1300" s="162"/>
+      <c r="E1300" s="162"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16397,9 +16401,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="161"/>
+      <c r="D1317" s="162"/>
+      <c r="E1317" s="162"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16550,9 +16554,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="161"/>
+      <c r="D1334" s="162"/>
+      <c r="E1334" s="162"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16703,9 +16707,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="161"/>
+      <c r="D1351" s="162"/>
+      <c r="E1351" s="162"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16856,18 +16860,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="176"/>
-      <c r="D1368" s="177"/>
-      <c r="E1368" s="177"/>
+      <c r="C1368" s="169"/>
+      <c r="D1368" s="170"/>
+      <c r="E1368" s="170"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="161"/>
+      <c r="D1369" s="162"/>
+      <c r="E1369" s="162"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17018,9 +17022,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="163"/>
+      <c r="D1386" s="164"/>
+      <c r="E1386" s="164"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17171,9 +17175,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="161"/>
+      <c r="D1403" s="162"/>
+      <c r="E1403" s="162"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17324,9 +17328,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="161"/>
+      <c r="D1420" s="162"/>
+      <c r="E1420" s="162"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17477,9 +17481,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="161"/>
+      <c r="D1437" s="162"/>
+      <c r="E1437" s="162"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17630,9 +17634,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="161"/>
+      <c r="D1454" s="162"/>
+      <c r="E1454" s="162"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17783,9 +17787,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="161"/>
+      <c r="D1471" s="162"/>
+      <c r="E1471" s="162"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17936,9 +17940,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="161"/>
+      <c r="D1488" s="162"/>
+      <c r="E1488" s="162"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18089,9 +18093,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="161"/>
+      <c r="D1505" s="162"/>
+      <c r="E1505" s="162"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18242,9 +18246,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="161"/>
+      <c r="D1522" s="162"/>
+      <c r="E1522" s="162"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18395,9 +18399,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="161"/>
+      <c r="D1539" s="162"/>
+      <c r="E1539" s="162"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18548,9 +18552,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="161"/>
+      <c r="D1556" s="162"/>
+      <c r="E1556" s="162"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18701,9 +18705,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="161"/>
+      <c r="D1573" s="162"/>
+      <c r="E1573" s="162"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18854,9 +18858,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="161"/>
+      <c r="D1590" s="162"/>
+      <c r="E1590" s="162"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19007,9 +19011,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="161"/>
+      <c r="D1607" s="162"/>
+      <c r="E1607" s="162"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19160,9 +19164,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="161"/>
+      <c r="D1624" s="162"/>
+      <c r="E1624" s="162"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19313,18 +19317,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="178"/>
-      <c r="D1641" s="179"/>
-      <c r="E1641" s="179"/>
+      <c r="C1641" s="167"/>
+      <c r="D1641" s="168"/>
+      <c r="E1641" s="168"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="161"/>
+      <c r="D1642" s="162"/>
+      <c r="E1642" s="162"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19475,9 +19479,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="163"/>
+      <c r="D1659" s="164"/>
+      <c r="E1659" s="164"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19628,9 +19632,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="161"/>
+      <c r="D1676" s="162"/>
+      <c r="E1676" s="162"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19781,9 +19785,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="161"/>
+      <c r="D1693" s="162"/>
+      <c r="E1693" s="162"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19934,9 +19938,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="161"/>
+      <c r="D1710" s="162"/>
+      <c r="E1710" s="162"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20087,9 +20091,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="161"/>
+      <c r="D1727" s="162"/>
+      <c r="E1727" s="162"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20240,9 +20244,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="161"/>
+      <c r="D1744" s="162"/>
+      <c r="E1744" s="162"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20393,9 +20397,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="161"/>
+      <c r="D1761" s="162"/>
+      <c r="E1761" s="162"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20546,9 +20550,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="161"/>
+      <c r="D1778" s="162"/>
+      <c r="E1778" s="162"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20699,9 +20703,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="161"/>
+      <c r="D1795" s="162"/>
+      <c r="E1795" s="162"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20852,9 +20856,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="161"/>
+      <c r="D1812" s="162"/>
+      <c r="E1812" s="162"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21005,9 +21009,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="161"/>
+      <c r="D1829" s="162"/>
+      <c r="E1829" s="162"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21158,9 +21162,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="161"/>
+      <c r="D1846" s="162"/>
+      <c r="E1846" s="162"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21311,9 +21315,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="161"/>
+      <c r="D1863" s="162"/>
+      <c r="E1863" s="162"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21464,9 +21468,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="161"/>
+      <c r="D1880" s="162"/>
+      <c r="E1880" s="162"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21617,9 +21621,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="161"/>
+      <c r="D1897" s="162"/>
+      <c r="E1897" s="162"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21770,18 +21774,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="180"/>
-      <c r="D1914" s="181"/>
-      <c r="E1914" s="181"/>
+      <c r="C1914" s="165"/>
+      <c r="D1914" s="166"/>
+      <c r="E1914" s="166"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="161"/>
+      <c r="D1915" s="162"/>
+      <c r="E1915" s="162"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21932,9 +21936,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="163"/>
+      <c r="D1932" s="164"/>
+      <c r="E1932" s="164"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22085,9 +22089,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="161"/>
+      <c r="D1949" s="162"/>
+      <c r="E1949" s="162"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22238,9 +22242,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="161"/>
+      <c r="D1966" s="162"/>
+      <c r="E1966" s="162"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22391,9 +22395,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="161"/>
+      <c r="D1983" s="162"/>
+      <c r="E1983" s="162"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22544,9 +22548,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="161"/>
+      <c r="D2000" s="162"/>
+      <c r="E2000" s="162"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22697,9 +22701,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="161"/>
+      <c r="D2017" s="162"/>
+      <c r="E2017" s="162"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22850,9 +22854,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="161"/>
+      <c r="D2034" s="162"/>
+      <c r="E2034" s="162"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23003,9 +23007,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="161"/>
+      <c r="D2051" s="162"/>
+      <c r="E2051" s="162"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23156,9 +23160,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="161"/>
+      <c r="D2068" s="162"/>
+      <c r="E2068" s="162"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23309,9 +23313,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="161"/>
+      <c r="D2085" s="162"/>
+      <c r="E2085" s="162"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23462,9 +23466,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="161"/>
+      <c r="D2102" s="162"/>
+      <c r="E2102" s="162"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23615,9 +23619,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="161"/>
+      <c r="D2119" s="162"/>
+      <c r="E2119" s="162"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23768,9 +23772,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="161"/>
+      <c r="D2136" s="162"/>
+      <c r="E2136" s="162"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23921,9 +23925,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="161"/>
+      <c r="D2153" s="162"/>
+      <c r="E2153" s="162"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24074,9 +24078,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="161"/>
+      <c r="D2170" s="162"/>
+      <c r="E2170" s="162"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24224,15 +24228,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24245,122 +24356,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25619,150 +25623,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="206" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="208"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="203" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="214"/>
+      <c r="B2" s="204"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="214"/>
+      <c r="B3" s="204"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="211"/>
-      <c r="B4" s="212"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="209" t="s">
+      <c r="A5" s="208" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="210"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="201" t="s">
+      <c r="A7" s="214" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="202"/>
+      <c r="B7" s="215"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="204"/>
+      <c r="B9" s="213"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="205"/>
-      <c r="B10" s="206"/>
+      <c r="A10" s="199"/>
+      <c r="B10" s="200"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="198"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="197" t="s">
+      <c r="A12" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="198"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="198"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="198"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="197" t="s">
+      <c r="A15" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="198"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="197" t="s">
+      <c r="A16" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="198"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="200"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="214" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="202"/>
+      <c r="B19" s="215"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="203" t="s">
+      <c r="A21" s="212" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="204"/>
+      <c r="B21" s="213"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="205"/>
-      <c r="B22" s="206"/>
+      <c r="A22" s="199"/>
+      <c r="B22" s="200"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="197" t="s">
+      <c r="A23" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="198"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="197"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="197" t="s">
+      <c r="A25" s="201" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="198"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="197" t="s">
+      <c r="A26" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="198"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25773,19 +25790,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Spiderman2 - saved final hostage (7 faster than before).  Afterwards though and interesting maneuver?  Is this a glitch?  I seem to only be able to do it by taking advantage of the dialog.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -2431,7 +2431,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2923,13 +2923,15 @@
       <c r="B29" s="150" t="s">
         <v>231</v>
       </c>
-      <c r="C29" s="101"/>
+      <c r="C29" s="101">
+        <v>3506</v>
+      </c>
       <c r="D29" s="101">
         <v>3713</v>
       </c>
       <c r="E29" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="F29" s="105"/>
     </row>

</xml_diff>

<commit_message>
Forgot to put this in with r957.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,7 +14,7 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2025,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2083,20 +2083,34 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2106,20 +2120,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2431,7 +2431,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2940,13 +2940,15 @@
       <c r="B30" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="101"/>
+      <c r="C30" s="101">
+        <v>4181</v>
+      </c>
       <c r="D30" s="101">
         <v>4463</v>
       </c>
       <c r="E30" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>282</v>
       </c>
       <c r="F30" s="105"/>
     </row>
@@ -4496,6 +4498,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4504,11 +4511,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4540,13 +4542,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4576,18 +4578,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4739,9 +4741,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4892,9 +4894,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5045,9 +5047,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="161"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5198,9 +5200,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="161"/>
-      <c r="D72" s="162"/>
-      <c r="E72" s="162"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5351,9 +5353,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="161"/>
-      <c r="D89" s="162"/>
-      <c r="E89" s="162"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5504,9 +5506,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="161"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5657,9 +5659,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="162"/>
-      <c r="E123" s="162"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5810,9 +5812,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="161"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="162"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5963,9 +5965,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="162"/>
-      <c r="E157" s="162"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6116,9 +6118,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="162"/>
-      <c r="E174" s="162"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6269,9 +6271,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="162"/>
-      <c r="E191" s="162"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6422,9 +6424,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="162"/>
-      <c r="E208" s="162"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6575,9 +6577,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="162"/>
-      <c r="E225" s="162"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6728,9 +6730,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="161"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6881,9 +6883,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="161"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7034,18 +7036,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="177"/>
-      <c r="D276" s="178"/>
-      <c r="E276" s="178"/>
+      <c r="C276" s="168"/>
+      <c r="D276" s="169"/>
+      <c r="E276" s="169"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="161"/>
-      <c r="D277" s="162"/>
-      <c r="E277" s="162"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7196,9 +7198,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="163"/>
-      <c r="D294" s="164"/>
-      <c r="E294" s="164"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7349,9 +7351,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="161"/>
-      <c r="D311" s="162"/>
-      <c r="E311" s="162"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7502,9 +7504,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="161"/>
-      <c r="D328" s="162"/>
-      <c r="E328" s="162"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7655,9 +7657,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="161"/>
-      <c r="D345" s="162"/>
-      <c r="E345" s="162"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7808,9 +7810,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="161"/>
-      <c r="D362" s="162"/>
-      <c r="E362" s="162"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7961,9 +7963,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="161"/>
-      <c r="D379" s="162"/>
-      <c r="E379" s="162"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8114,9 +8116,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="161"/>
-      <c r="D396" s="162"/>
-      <c r="E396" s="162"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8267,9 +8269,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="161"/>
-      <c r="D413" s="162"/>
-      <c r="E413" s="162"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8420,9 +8422,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="161"/>
-      <c r="D430" s="162"/>
-      <c r="E430" s="162"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8573,9 +8575,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="161"/>
-      <c r="D447" s="162"/>
-      <c r="E447" s="162"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8726,9 +8728,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="161"/>
-      <c r="D464" s="162"/>
-      <c r="E464" s="162"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8879,9 +8881,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="161"/>
-      <c r="D481" s="162"/>
-      <c r="E481" s="162"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9032,9 +9034,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="161"/>
-      <c r="D498" s="162"/>
-      <c r="E498" s="162"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9185,9 +9187,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="161"/>
-      <c r="D515" s="162"/>
-      <c r="E515" s="162"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9338,9 +9340,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="161"/>
-      <c r="D532" s="162"/>
-      <c r="E532" s="162"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9491,18 +9493,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="170"/>
+      <c r="D549" s="171"/>
+      <c r="E549" s="171"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="161"/>
-      <c r="D550" s="162"/>
-      <c r="E550" s="162"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9653,9 +9655,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="163"/>
-      <c r="D567" s="164"/>
-      <c r="E567" s="164"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9806,9 +9808,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="161"/>
-      <c r="D584" s="162"/>
-      <c r="E584" s="162"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9959,9 +9961,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="161"/>
-      <c r="D601" s="162"/>
-      <c r="E601" s="162"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10112,9 +10114,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="161"/>
-      <c r="D618" s="162"/>
-      <c r="E618" s="162"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10265,9 +10267,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="161"/>
-      <c r="D635" s="162"/>
-      <c r="E635" s="162"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10418,9 +10420,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="161"/>
-      <c r="D652" s="162"/>
-      <c r="E652" s="162"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10571,9 +10573,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="161"/>
-      <c r="D669" s="162"/>
-      <c r="E669" s="162"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10724,9 +10726,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="161"/>
-      <c r="D686" s="162"/>
-      <c r="E686" s="162"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10877,9 +10879,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="161"/>
-      <c r="D703" s="162"/>
-      <c r="E703" s="162"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11030,9 +11032,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="161"/>
-      <c r="D720" s="162"/>
-      <c r="E720" s="162"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11183,9 +11185,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="161"/>
-      <c r="D737" s="162"/>
-      <c r="E737" s="162"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11336,9 +11338,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="161"/>
-      <c r="D754" s="162"/>
-      <c r="E754" s="162"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11489,9 +11491,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="161"/>
-      <c r="D771" s="162"/>
-      <c r="E771" s="162"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11642,9 +11644,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="161"/>
-      <c r="D788" s="162"/>
-      <c r="E788" s="162"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11795,9 +11797,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="161"/>
-      <c r="D805" s="162"/>
-      <c r="E805" s="162"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11948,18 +11950,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="173"/>
-      <c r="D822" s="174"/>
-      <c r="E822" s="174"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="161"/>
-      <c r="D823" s="162"/>
-      <c r="E823" s="162"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12110,9 +12112,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="163"/>
-      <c r="D840" s="164"/>
-      <c r="E840" s="164"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12263,9 +12265,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="161"/>
-      <c r="D857" s="162"/>
-      <c r="E857" s="162"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12416,9 +12418,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="161"/>
-      <c r="D874" s="162"/>
-      <c r="E874" s="162"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12569,9 +12571,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="161"/>
-      <c r="D891" s="162"/>
-      <c r="E891" s="162"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12722,9 +12724,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="161"/>
-      <c r="D908" s="162"/>
-      <c r="E908" s="162"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12875,9 +12877,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="161"/>
-      <c r="D925" s="162"/>
-      <c r="E925" s="162"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13028,9 +13030,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="161"/>
-      <c r="D942" s="162"/>
-      <c r="E942" s="162"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13181,9 +13183,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="161"/>
-      <c r="D959" s="162"/>
-      <c r="E959" s="162"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13334,9 +13336,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="161"/>
-      <c r="D976" s="162"/>
-      <c r="E976" s="162"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13487,9 +13489,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="161"/>
-      <c r="D993" s="162"/>
-      <c r="E993" s="162"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13640,9 +13642,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="161"/>
-      <c r="D1010" s="162"/>
-      <c r="E1010" s="162"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13793,9 +13795,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="161"/>
-      <c r="D1027" s="162"/>
-      <c r="E1027" s="162"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13946,9 +13948,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="161"/>
-      <c r="D1044" s="162"/>
-      <c r="E1044" s="162"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14099,9 +14101,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="161"/>
-      <c r="D1061" s="162"/>
-      <c r="E1061" s="162"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14252,9 +14254,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="161"/>
-      <c r="D1078" s="162"/>
-      <c r="E1078" s="162"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14405,18 +14407,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="171"/>
-      <c r="D1095" s="172"/>
-      <c r="E1095" s="172"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="161"/>
-      <c r="D1096" s="162"/>
-      <c r="E1096" s="162"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14567,9 +14569,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="163"/>
-      <c r="D1113" s="164"/>
-      <c r="E1113" s="164"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14720,9 +14722,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="161"/>
-      <c r="D1130" s="162"/>
-      <c r="E1130" s="162"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14873,9 +14875,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="161"/>
-      <c r="D1147" s="162"/>
-      <c r="E1147" s="162"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15026,9 +15028,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="161"/>
-      <c r="D1164" s="162"/>
-      <c r="E1164" s="162"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15179,9 +15181,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="161"/>
-      <c r="D1181" s="162"/>
-      <c r="E1181" s="162"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15332,9 +15334,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="161"/>
-      <c r="D1198" s="162"/>
-      <c r="E1198" s="162"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15485,9 +15487,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="161"/>
-      <c r="D1215" s="162"/>
-      <c r="E1215" s="162"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15638,9 +15640,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="161"/>
-      <c r="D1232" s="162"/>
-      <c r="E1232" s="162"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15791,9 +15793,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="161"/>
-      <c r="D1249" s="162"/>
-      <c r="E1249" s="162"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15944,9 +15946,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="161"/>
-      <c r="D1266" s="162"/>
-      <c r="E1266" s="162"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16097,9 +16099,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="161"/>
-      <c r="D1283" s="162"/>
-      <c r="E1283" s="162"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16250,9 +16252,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="161"/>
-      <c r="D1300" s="162"/>
-      <c r="E1300" s="162"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16403,9 +16405,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="161"/>
-      <c r="D1317" s="162"/>
-      <c r="E1317" s="162"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16556,9 +16558,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="161"/>
-      <c r="D1334" s="162"/>
-      <c r="E1334" s="162"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16709,9 +16711,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="161"/>
-      <c r="D1351" s="162"/>
-      <c r="E1351" s="162"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16862,18 +16864,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="169"/>
-      <c r="D1368" s="170"/>
-      <c r="E1368" s="170"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="161"/>
-      <c r="D1369" s="162"/>
-      <c r="E1369" s="162"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17024,9 +17026,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="163"/>
-      <c r="D1386" s="164"/>
-      <c r="E1386" s="164"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17177,9 +17179,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="161"/>
-      <c r="D1403" s="162"/>
-      <c r="E1403" s="162"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17330,9 +17332,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="161"/>
-      <c r="D1420" s="162"/>
-      <c r="E1420" s="162"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17483,9 +17485,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="161"/>
-      <c r="D1437" s="162"/>
-      <c r="E1437" s="162"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17636,9 +17638,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="161"/>
-      <c r="D1454" s="162"/>
-      <c r="E1454" s="162"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17789,9 +17791,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="161"/>
-      <c r="D1471" s="162"/>
-      <c r="E1471" s="162"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17942,9 +17944,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="161"/>
-      <c r="D1488" s="162"/>
-      <c r="E1488" s="162"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18095,9 +18097,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="161"/>
-      <c r="D1505" s="162"/>
-      <c r="E1505" s="162"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18248,9 +18250,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="161"/>
-      <c r="D1522" s="162"/>
-      <c r="E1522" s="162"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18401,9 +18403,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="161"/>
-      <c r="D1539" s="162"/>
-      <c r="E1539" s="162"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18554,9 +18556,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="161"/>
-      <c r="D1556" s="162"/>
-      <c r="E1556" s="162"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18707,9 +18709,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="161"/>
-      <c r="D1573" s="162"/>
-      <c r="E1573" s="162"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18860,9 +18862,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="161"/>
-      <c r="D1590" s="162"/>
-      <c r="E1590" s="162"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19013,9 +19015,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="161"/>
-      <c r="D1607" s="162"/>
-      <c r="E1607" s="162"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19166,9 +19168,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="161"/>
-      <c r="D1624" s="162"/>
-      <c r="E1624" s="162"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19319,18 +19321,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="167"/>
-      <c r="D1641" s="168"/>
-      <c r="E1641" s="168"/>
+      <c r="C1641" s="178"/>
+      <c r="D1641" s="179"/>
+      <c r="E1641" s="179"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="161"/>
-      <c r="D1642" s="162"/>
-      <c r="E1642" s="162"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19481,9 +19483,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="163"/>
-      <c r="D1659" s="164"/>
-      <c r="E1659" s="164"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19634,9 +19636,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="161"/>
-      <c r="D1676" s="162"/>
-      <c r="E1676" s="162"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19787,9 +19789,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="161"/>
-      <c r="D1693" s="162"/>
-      <c r="E1693" s="162"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19940,9 +19942,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="161"/>
-      <c r="D1710" s="162"/>
-      <c r="E1710" s="162"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20093,9 +20095,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="161"/>
-      <c r="D1727" s="162"/>
-      <c r="E1727" s="162"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20246,9 +20248,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="161"/>
-      <c r="D1744" s="162"/>
-      <c r="E1744" s="162"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20399,9 +20401,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="161"/>
-      <c r="D1761" s="162"/>
-      <c r="E1761" s="162"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20552,9 +20554,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="161"/>
-      <c r="D1778" s="162"/>
-      <c r="E1778" s="162"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20705,9 +20707,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="161"/>
-      <c r="D1795" s="162"/>
-      <c r="E1795" s="162"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20858,9 +20860,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="161"/>
-      <c r="D1812" s="162"/>
-      <c r="E1812" s="162"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21011,9 +21013,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="161"/>
-      <c r="D1829" s="162"/>
-      <c r="E1829" s="162"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21164,9 +21166,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="161"/>
-      <c r="D1846" s="162"/>
-      <c r="E1846" s="162"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21317,9 +21319,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="161"/>
-      <c r="D1863" s="162"/>
-      <c r="E1863" s="162"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21470,9 +21472,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="161"/>
-      <c r="D1880" s="162"/>
-      <c r="E1880" s="162"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21623,9 +21625,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="161"/>
-      <c r="D1897" s="162"/>
-      <c r="E1897" s="162"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21776,18 +21778,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="165"/>
-      <c r="D1914" s="166"/>
-      <c r="E1914" s="166"/>
+      <c r="C1914" s="180"/>
+      <c r="D1914" s="181"/>
+      <c r="E1914" s="181"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="161"/>
-      <c r="D1915" s="162"/>
-      <c r="E1915" s="162"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21938,9 +21940,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="163"/>
-      <c r="D1932" s="164"/>
-      <c r="E1932" s="164"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22091,9 +22093,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="161"/>
-      <c r="D1949" s="162"/>
-      <c r="E1949" s="162"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22244,9 +22246,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="161"/>
-      <c r="D1966" s="162"/>
-      <c r="E1966" s="162"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22397,9 +22399,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="161"/>
-      <c r="D1983" s="162"/>
-      <c r="E1983" s="162"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22550,9 +22552,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="161"/>
-      <c r="D2000" s="162"/>
-      <c r="E2000" s="162"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22703,9 +22705,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="161"/>
-      <c r="D2017" s="162"/>
-      <c r="E2017" s="162"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22856,9 +22858,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="161"/>
-      <c r="D2034" s="162"/>
-      <c r="E2034" s="162"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23009,9 +23011,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="161"/>
-      <c r="D2051" s="162"/>
-      <c r="E2051" s="162"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23162,9 +23164,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="161"/>
-      <c r="D2068" s="162"/>
-      <c r="E2068" s="162"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23315,9 +23317,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="161"/>
-      <c r="D2085" s="162"/>
-      <c r="E2085" s="162"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23468,9 +23470,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="161"/>
-      <c r="D2102" s="162"/>
-      <c r="E2102" s="162"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23621,9 +23623,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="161"/>
-      <c r="D2119" s="162"/>
-      <c r="E2119" s="162"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23774,9 +23776,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="161"/>
-      <c r="D2136" s="162"/>
-      <c r="E2136" s="162"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23927,9 +23929,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="161"/>
-      <c r="D2153" s="162"/>
-      <c r="E2153" s="162"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24080,9 +24082,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="161"/>
-      <c r="D2170" s="162"/>
-      <c r="E2170" s="162"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24230,26 +24232,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24262,111 +24349,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25625,163 +25627,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="207"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="215" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="204"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="210"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="208" t="s">
+      <c r="A5" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="209"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="214" t="s">
+      <c r="A7" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="215"/>
+      <c r="B7" s="202"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="203" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="213"/>
+      <c r="B9" s="204"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="206"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="197" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="214" t="s">
+      <c r="A19" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="215"/>
+      <c r="B19" s="202"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="203" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="213"/>
+      <c r="B21" s="204"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="199"/>
-      <c r="B22" s="200"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="206"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25792,6 +25781,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Spiderman2 - Next 2 convicts killed and up to the one after that.  However, I hope we can find a faster way up the wall there.  Also removed the compare .dsm since we are past my original wip now.
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,7 +14,7 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -2025,29 +2025,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2083,34 +2083,20 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2120,6 +2106,20 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,8 +2430,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2985,13 +2985,15 @@
       <c r="B33" s="150" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="101"/>
+      <c r="C33" s="101">
+        <v>5092</v>
+      </c>
       <c r="D33" s="101">
         <v>5392</v>
       </c>
       <c r="E33" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F33" s="105"/>
     </row>
@@ -3000,13 +3002,15 @@
       <c r="B34" s="150" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="101"/>
+      <c r="C34" s="101">
+        <v>5142</v>
+      </c>
       <c r="D34" s="101">
         <v>5443</v>
       </c>
       <c r="E34" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="F34" s="105"/>
     </row>
@@ -3015,13 +3019,15 @@
       <c r="B35" s="150" t="s">
         <v>235</v>
       </c>
-      <c r="C35" s="101"/>
+      <c r="C35" s="101">
+        <v>5434</v>
+      </c>
       <c r="D35" s="101">
         <v>5819</v>
       </c>
       <c r="E35" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F35" s="105"/>
     </row>
@@ -3030,13 +3036,15 @@
       <c r="B36" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="99"/>
+      <c r="C36" s="99">
+        <v>5434</v>
+      </c>
       <c r="D36" s="99">
         <v>5819</v>
       </c>
       <c r="E36" s="125">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F36" s="104"/>
     </row>
@@ -3049,7 +3057,7 @@
       </c>
       <c r="C37" s="103">
         <f>C36-C20</f>
-        <v>-1001</v>
+        <v>4433</v>
       </c>
       <c r="D37" s="103">
         <f>D36-D20</f>
@@ -3057,12 +3065,12 @@
       </c>
       <c r="E37" s="126">
         <f>E36-E20</f>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F37" s="108"/>
       <c r="G37" s="112">
         <f>E37</f>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1"/>
@@ -3091,13 +3099,15 @@
       <c r="B40" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="C40" s="99"/>
+      <c r="C40" s="99">
+        <v>5434</v>
+      </c>
       <c r="D40" s="99">
         <v>5819</v>
       </c>
       <c r="E40" s="123">
         <f t="shared" ref="E40:E53" si="3">IF(AND(C40&gt;0,D40&gt;0), D40-C40, 0)</f>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F40" s="104"/>
     </row>
@@ -3106,13 +3116,15 @@
       <c r="B41" s="150" t="s">
         <v>221</v>
       </c>
-      <c r="C41" s="101"/>
+      <c r="C41" s="101">
+        <v>5434</v>
+      </c>
       <c r="D41" s="101">
         <v>5819</v>
       </c>
       <c r="E41" s="124">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F41" s="105"/>
     </row>
@@ -3259,7 +3271,7 @@
       </c>
       <c r="C54" s="103">
         <f>C53-C40</f>
-        <v>0</v>
+        <v>-5434</v>
       </c>
       <c r="D54" s="103">
         <f>D53-D40</f>
@@ -3267,12 +3279,12 @@
       </c>
       <c r="E54" s="126">
         <f>E53-E40</f>
-        <v>0</v>
+        <v>-385</v>
       </c>
       <c r="F54" s="107"/>
       <c r="G54" s="112">
         <f>E54</f>
-        <v>0</v>
+        <v>-385</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="13.5" thickBot="1"/>
@@ -4498,11 +4510,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4511,6 +4518,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4542,13 +4554,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4578,18 +4590,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4741,9 +4753,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4894,9 +4906,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="161"/>
+      <c r="D38" s="162"/>
+      <c r="E38" s="162"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5047,9 +5059,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="161"/>
+      <c r="D55" s="162"/>
+      <c r="E55" s="162"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5200,9 +5212,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="161"/>
+      <c r="D72" s="162"/>
+      <c r="E72" s="162"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5353,9 +5365,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="161"/>
+      <c r="D89" s="162"/>
+      <c r="E89" s="162"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5506,9 +5518,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="161"/>
+      <c r="D106" s="162"/>
+      <c r="E106" s="162"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5659,9 +5671,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="161"/>
+      <c r="D123" s="162"/>
+      <c r="E123" s="162"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5812,9 +5824,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="161"/>
+      <c r="D140" s="162"/>
+      <c r="E140" s="162"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5965,9 +5977,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="161"/>
+      <c r="D157" s="162"/>
+      <c r="E157" s="162"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6118,9 +6130,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="161"/>
+      <c r="D174" s="162"/>
+      <c r="E174" s="162"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6271,9 +6283,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="161"/>
+      <c r="D191" s="162"/>
+      <c r="E191" s="162"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6424,9 +6436,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="161"/>
+      <c r="D208" s="162"/>
+      <c r="E208" s="162"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6577,9 +6589,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="161"/>
+      <c r="D225" s="162"/>
+      <c r="E225" s="162"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6730,9 +6742,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="161"/>
+      <c r="D242" s="162"/>
+      <c r="E242" s="162"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6883,9 +6895,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="161"/>
+      <c r="D259" s="162"/>
+      <c r="E259" s="162"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7036,18 +7048,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="168"/>
-      <c r="D276" s="169"/>
-      <c r="E276" s="169"/>
+      <c r="C276" s="177"/>
+      <c r="D276" s="178"/>
+      <c r="E276" s="178"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="161"/>
+      <c r="D277" s="162"/>
+      <c r="E277" s="162"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7198,9 +7210,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="163"/>
+      <c r="D294" s="164"/>
+      <c r="E294" s="164"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7351,9 +7363,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="161"/>
+      <c r="D311" s="162"/>
+      <c r="E311" s="162"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7504,9 +7516,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="161"/>
+      <c r="D328" s="162"/>
+      <c r="E328" s="162"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7657,9 +7669,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="161"/>
+      <c r="D345" s="162"/>
+      <c r="E345" s="162"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7810,9 +7822,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="161"/>
+      <c r="D362" s="162"/>
+      <c r="E362" s="162"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7963,9 +7975,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="161"/>
+      <c r="D379" s="162"/>
+      <c r="E379" s="162"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8116,9 +8128,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="161"/>
+      <c r="D396" s="162"/>
+      <c r="E396" s="162"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8269,9 +8281,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="161"/>
+      <c r="D413" s="162"/>
+      <c r="E413" s="162"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8422,9 +8434,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="161"/>
+      <c r="D430" s="162"/>
+      <c r="E430" s="162"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8575,9 +8587,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="161"/>
+      <c r="D447" s="162"/>
+      <c r="E447" s="162"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8728,9 +8740,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="161"/>
+      <c r="D464" s="162"/>
+      <c r="E464" s="162"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8881,9 +8893,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="161"/>
+      <c r="D481" s="162"/>
+      <c r="E481" s="162"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9034,9 +9046,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="161"/>
+      <c r="D498" s="162"/>
+      <c r="E498" s="162"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9187,9 +9199,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="161"/>
+      <c r="D515" s="162"/>
+      <c r="E515" s="162"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9340,9 +9352,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="161"/>
+      <c r="D532" s="162"/>
+      <c r="E532" s="162"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9493,18 +9505,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="170"/>
-      <c r="D549" s="171"/>
-      <c r="E549" s="171"/>
+      <c r="C549" s="175"/>
+      <c r="D549" s="176"/>
+      <c r="E549" s="176"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="161"/>
+      <c r="D550" s="162"/>
+      <c r="E550" s="162"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9655,9 +9667,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="163"/>
+      <c r="D567" s="164"/>
+      <c r="E567" s="164"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9808,9 +9820,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="161"/>
+      <c r="D584" s="162"/>
+      <c r="E584" s="162"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9961,9 +9973,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="161"/>
+      <c r="D601" s="162"/>
+      <c r="E601" s="162"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10114,9 +10126,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="161"/>
+      <c r="D618" s="162"/>
+      <c r="E618" s="162"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10267,9 +10279,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="161"/>
+      <c r="D635" s="162"/>
+      <c r="E635" s="162"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10420,9 +10432,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="161"/>
+      <c r="D652" s="162"/>
+      <c r="E652" s="162"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10573,9 +10585,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="161"/>
+      <c r="D669" s="162"/>
+      <c r="E669" s="162"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10726,9 +10738,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="161"/>
+      <c r="D686" s="162"/>
+      <c r="E686" s="162"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10879,9 +10891,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="161"/>
+      <c r="D703" s="162"/>
+      <c r="E703" s="162"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11032,9 +11044,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="161"/>
+      <c r="D720" s="162"/>
+      <c r="E720" s="162"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11185,9 +11197,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="161"/>
+      <c r="D737" s="162"/>
+      <c r="E737" s="162"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11338,9 +11350,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="161"/>
+      <c r="D754" s="162"/>
+      <c r="E754" s="162"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11491,9 +11503,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="161"/>
+      <c r="D771" s="162"/>
+      <c r="E771" s="162"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11644,9 +11656,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="161"/>
+      <c r="D788" s="162"/>
+      <c r="E788" s="162"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11797,9 +11809,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="161"/>
+      <c r="D805" s="162"/>
+      <c r="E805" s="162"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11950,18 +11962,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="172"/>
-      <c r="D822" s="173"/>
-      <c r="E822" s="173"/>
+      <c r="C822" s="173"/>
+      <c r="D822" s="174"/>
+      <c r="E822" s="174"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="161"/>
+      <c r="D823" s="162"/>
+      <c r="E823" s="162"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12112,9 +12124,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="163"/>
+      <c r="D840" s="164"/>
+      <c r="E840" s="164"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12265,9 +12277,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="161"/>
+      <c r="D857" s="162"/>
+      <c r="E857" s="162"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12418,9 +12430,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="161"/>
+      <c r="D874" s="162"/>
+      <c r="E874" s="162"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12571,9 +12583,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="161"/>
+      <c r="D891" s="162"/>
+      <c r="E891" s="162"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12724,9 +12736,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="161"/>
+      <c r="D908" s="162"/>
+      <c r="E908" s="162"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12877,9 +12889,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="161"/>
+      <c r="D925" s="162"/>
+      <c r="E925" s="162"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13030,9 +13042,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="161"/>
+      <c r="D942" s="162"/>
+      <c r="E942" s="162"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13183,9 +13195,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="161"/>
+      <c r="D959" s="162"/>
+      <c r="E959" s="162"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13336,9 +13348,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="161"/>
+      <c r="D976" s="162"/>
+      <c r="E976" s="162"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13489,9 +13501,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="161"/>
+      <c r="D993" s="162"/>
+      <c r="E993" s="162"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13642,9 +13654,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="161"/>
+      <c r="D1010" s="162"/>
+      <c r="E1010" s="162"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13795,9 +13807,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="161"/>
+      <c r="D1027" s="162"/>
+      <c r="E1027" s="162"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13948,9 +13960,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="161"/>
+      <c r="D1044" s="162"/>
+      <c r="E1044" s="162"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14101,9 +14113,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="161"/>
+      <c r="D1061" s="162"/>
+      <c r="E1061" s="162"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14254,9 +14266,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="161"/>
+      <c r="D1078" s="162"/>
+      <c r="E1078" s="162"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14407,18 +14419,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="171"/>
+      <c r="D1095" s="172"/>
+      <c r="E1095" s="172"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="161"/>
+      <c r="D1096" s="162"/>
+      <c r="E1096" s="162"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14569,9 +14581,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="163"/>
+      <c r="D1113" s="164"/>
+      <c r="E1113" s="164"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14722,9 +14734,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="161"/>
+      <c r="D1130" s="162"/>
+      <c r="E1130" s="162"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14875,9 +14887,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="161"/>
+      <c r="D1147" s="162"/>
+      <c r="E1147" s="162"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15028,9 +15040,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="161"/>
+      <c r="D1164" s="162"/>
+      <c r="E1164" s="162"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15181,9 +15193,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="161"/>
+      <c r="D1181" s="162"/>
+      <c r="E1181" s="162"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15334,9 +15346,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="161"/>
+      <c r="D1198" s="162"/>
+      <c r="E1198" s="162"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15487,9 +15499,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="161"/>
+      <c r="D1215" s="162"/>
+      <c r="E1215" s="162"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15640,9 +15652,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="161"/>
+      <c r="D1232" s="162"/>
+      <c r="E1232" s="162"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15793,9 +15805,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="161"/>
+      <c r="D1249" s="162"/>
+      <c r="E1249" s="162"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15946,9 +15958,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="161"/>
+      <c r="D1266" s="162"/>
+      <c r="E1266" s="162"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16099,9 +16111,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="161"/>
+      <c r="D1283" s="162"/>
+      <c r="E1283" s="162"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16252,9 +16264,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="161"/>
+      <c r="D1300" s="162"/>
+      <c r="E1300" s="162"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16405,9 +16417,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="161"/>
+      <c r="D1317" s="162"/>
+      <c r="E1317" s="162"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16558,9 +16570,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="161"/>
+      <c r="D1334" s="162"/>
+      <c r="E1334" s="162"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16711,9 +16723,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="161"/>
+      <c r="D1351" s="162"/>
+      <c r="E1351" s="162"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16864,18 +16876,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="176"/>
-      <c r="D1368" s="177"/>
-      <c r="E1368" s="177"/>
+      <c r="C1368" s="169"/>
+      <c r="D1368" s="170"/>
+      <c r="E1368" s="170"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="161"/>
+      <c r="D1369" s="162"/>
+      <c r="E1369" s="162"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17026,9 +17038,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="163"/>
+      <c r="D1386" s="164"/>
+      <c r="E1386" s="164"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17179,9 +17191,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="161"/>
+      <c r="D1403" s="162"/>
+      <c r="E1403" s="162"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17332,9 +17344,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="161"/>
+      <c r="D1420" s="162"/>
+      <c r="E1420" s="162"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17485,9 +17497,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="161"/>
+      <c r="D1437" s="162"/>
+      <c r="E1437" s="162"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17638,9 +17650,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="161"/>
+      <c r="D1454" s="162"/>
+      <c r="E1454" s="162"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17791,9 +17803,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="161"/>
+      <c r="D1471" s="162"/>
+      <c r="E1471" s="162"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17944,9 +17956,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="161"/>
+      <c r="D1488" s="162"/>
+      <c r="E1488" s="162"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18097,9 +18109,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="161"/>
+      <c r="D1505" s="162"/>
+      <c r="E1505" s="162"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18250,9 +18262,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="161"/>
+      <c r="D1522" s="162"/>
+      <c r="E1522" s="162"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18403,9 +18415,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="161"/>
+      <c r="D1539" s="162"/>
+      <c r="E1539" s="162"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18556,9 +18568,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="161"/>
+      <c r="D1556" s="162"/>
+      <c r="E1556" s="162"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18709,9 +18721,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="161"/>
+      <c r="D1573" s="162"/>
+      <c r="E1573" s="162"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18862,9 +18874,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="161"/>
+      <c r="D1590" s="162"/>
+      <c r="E1590" s="162"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19015,9 +19027,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="161"/>
+      <c r="D1607" s="162"/>
+      <c r="E1607" s="162"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19168,9 +19180,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="161"/>
+      <c r="D1624" s="162"/>
+      <c r="E1624" s="162"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19321,18 +19333,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="178"/>
-      <c r="D1641" s="179"/>
-      <c r="E1641" s="179"/>
+      <c r="C1641" s="167"/>
+      <c r="D1641" s="168"/>
+      <c r="E1641" s="168"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="161"/>
+      <c r="D1642" s="162"/>
+      <c r="E1642" s="162"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19483,9 +19495,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="163"/>
+      <c r="D1659" s="164"/>
+      <c r="E1659" s="164"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19636,9 +19648,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="161"/>
+      <c r="D1676" s="162"/>
+      <c r="E1676" s="162"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19789,9 +19801,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="161"/>
+      <c r="D1693" s="162"/>
+      <c r="E1693" s="162"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19942,9 +19954,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="161"/>
+      <c r="D1710" s="162"/>
+      <c r="E1710" s="162"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20095,9 +20107,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="161"/>
+      <c r="D1727" s="162"/>
+      <c r="E1727" s="162"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20248,9 +20260,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="161"/>
+      <c r="D1744" s="162"/>
+      <c r="E1744" s="162"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20401,9 +20413,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="161"/>
+      <c r="D1761" s="162"/>
+      <c r="E1761" s="162"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20554,9 +20566,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="161"/>
+      <c r="D1778" s="162"/>
+      <c r="E1778" s="162"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20707,9 +20719,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="161"/>
+      <c r="D1795" s="162"/>
+      <c r="E1795" s="162"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20860,9 +20872,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="161"/>
+      <c r="D1812" s="162"/>
+      <c r="E1812" s="162"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21013,9 +21025,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="161"/>
+      <c r="D1829" s="162"/>
+      <c r="E1829" s="162"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21166,9 +21178,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="161"/>
+      <c r="D1846" s="162"/>
+      <c r="E1846" s="162"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21319,9 +21331,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="161"/>
+      <c r="D1863" s="162"/>
+      <c r="E1863" s="162"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21472,9 +21484,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="161"/>
+      <c r="D1880" s="162"/>
+      <c r="E1880" s="162"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21625,9 +21637,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="161"/>
+      <c r="D1897" s="162"/>
+      <c r="E1897" s="162"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21778,18 +21790,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="180"/>
-      <c r="D1914" s="181"/>
-      <c r="E1914" s="181"/>
+      <c r="C1914" s="165"/>
+      <c r="D1914" s="166"/>
+      <c r="E1914" s="166"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="161"/>
+      <c r="D1915" s="162"/>
+      <c r="E1915" s="162"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21940,9 +21952,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="163"/>
+      <c r="D1932" s="164"/>
+      <c r="E1932" s="164"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22093,9 +22105,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="161"/>
+      <c r="D1949" s="162"/>
+      <c r="E1949" s="162"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22246,9 +22258,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="161"/>
+      <c r="D1966" s="162"/>
+      <c r="E1966" s="162"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22399,9 +22411,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="161"/>
+      <c r="D1983" s="162"/>
+      <c r="E1983" s="162"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22552,9 +22564,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="161"/>
+      <c r="D2000" s="162"/>
+      <c r="E2000" s="162"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22705,9 +22717,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="161"/>
+      <c r="D2017" s="162"/>
+      <c r="E2017" s="162"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22858,9 +22870,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="161"/>
+      <c r="D2034" s="162"/>
+      <c r="E2034" s="162"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23011,9 +23023,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="161"/>
+      <c r="D2051" s="162"/>
+      <c r="E2051" s="162"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23164,9 +23176,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="161"/>
+      <c r="D2068" s="162"/>
+      <c r="E2068" s="162"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23317,9 +23329,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="161"/>
+      <c r="D2085" s="162"/>
+      <c r="E2085" s="162"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23470,9 +23482,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="161"/>
+      <c r="D2102" s="162"/>
+      <c r="E2102" s="162"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23623,9 +23635,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="161"/>
+      <c r="D2119" s="162"/>
+      <c r="E2119" s="162"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23776,9 +23788,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="161"/>
+      <c r="D2136" s="162"/>
+      <c r="E2136" s="162"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23929,9 +23941,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="161"/>
+      <c r="D2153" s="162"/>
+      <c r="E2153" s="162"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24082,9 +24094,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="161"/>
+      <c r="D2170" s="162"/>
+      <c r="E2170" s="162"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24232,15 +24244,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24253,122 +24372,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25627,150 +25639,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="206" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="208"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="203" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="214"/>
+      <c r="B2" s="204"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="214"/>
+      <c r="B3" s="204"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="211"/>
-      <c r="B4" s="212"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="209" t="s">
+      <c r="A5" s="208" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="210"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="201" t="s">
+      <c r="A7" s="214" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="202"/>
+      <c r="B7" s="215"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="204"/>
+      <c r="B9" s="213"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="205"/>
-      <c r="B10" s="206"/>
+      <c r="A10" s="199"/>
+      <c r="B10" s="200"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="198"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="197" t="s">
+      <c r="A12" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="198"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="198"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="198"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="197" t="s">
+      <c r="A15" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="198"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="197" t="s">
+      <c r="A16" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="198"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="200"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="214" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="202"/>
+      <c r="B19" s="215"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="203" t="s">
+      <c r="A21" s="212" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="204"/>
+      <c r="B21" s="213"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="205"/>
-      <c r="B22" s="206"/>
+      <c r="A22" s="199"/>
+      <c r="B22" s="200"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="197" t="s">
+      <c r="A23" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="198"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="197"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="197" t="s">
+      <c r="A25" s="201" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="198"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="197" t="s">
+      <c r="A26" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="198"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25781,19 +25806,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Spider-man 2 - Level 3 begin
</commit_message>
<xml_diff>
--- a/Spiderman2/Spider2.xlsx
+++ b/Spiderman2/Spider2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="237">
   <si>
     <t>Notes</t>
   </si>
@@ -768,6 +768,9 @@
   <si>
     <t>1st Move level 2</t>
   </si>
+  <si>
+    <t>End level</t>
+  </si>
 </sst>
 </file>
 
@@ -777,10 +780,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1712,34 +1722,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1747,208 +1757,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1958,10 +1968,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1982,144 +1992,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2430,8 +2443,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="6" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -3240,9 +3253,13 @@
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1">
       <c r="A52" s="153"/>
-      <c r="B52" s="100"/>
+      <c r="B52" s="216" t="s">
+        <v>236</v>
+      </c>
       <c r="C52" s="101"/>
-      <c r="D52" s="101"/>
+      <c r="D52" s="101">
+        <v>9428</v>
+      </c>
       <c r="E52" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3288,7 +3305,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="56" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="56" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
       <c r="A56" s="154" t="s">
         <v>170</v>
       </c>
@@ -3308,20 +3325,22 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="57" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A57" s="153"/>
       <c r="B57" s="98" t="s">
         <v>183</v>
       </c>
       <c r="C57" s="99"/>
-      <c r="D57" s="99"/>
+      <c r="D57" s="99">
+        <v>9746</v>
+      </c>
       <c r="E57" s="123">
         <f t="shared" ref="E57:E70" si="4">IF(AND(C57&gt;0,D57&gt;0), D57-C57, 0)</f>
         <v>0</v>
       </c>
       <c r="F57" s="104"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
+    <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A58" s="153"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
@@ -3332,7 +3351,7 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="59" spans="1:7" ht="15" outlineLevel="1">
       <c r="A59" s="153"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
@@ -3343,7 +3362,7 @@
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="60" spans="1:7" ht="15" outlineLevel="1">
       <c r="A60" s="153"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
@@ -3354,7 +3373,7 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="61" spans="1:7" ht="15" outlineLevel="1">
       <c r="A61" s="153"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
@@ -3365,7 +3384,7 @@
       </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="62" spans="1:7" ht="15" outlineLevel="1">
       <c r="A62" s="153"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
@@ -3376,7 +3395,7 @@
       </c>
       <c r="F62" s="105"/>
     </row>
-    <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="63" spans="1:7" ht="15" outlineLevel="1">
       <c r="A63" s="153"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
@@ -3387,7 +3406,7 @@
       </c>
       <c r="F63" s="105"/>
     </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="64" spans="1:7" ht="15" outlineLevel="1">
       <c r="A64" s="153"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
@@ -3398,7 +3417,7 @@
       </c>
       <c r="F64" s="105"/>
     </row>
-    <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="65" spans="1:7" ht="15" outlineLevel="1">
       <c r="A65" s="153"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
@@ -3409,7 +3428,7 @@
       </c>
       <c r="F65" s="105"/>
     </row>
-    <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="66" spans="1:7" ht="15" outlineLevel="1">
       <c r="A66" s="153"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
@@ -3420,7 +3439,7 @@
       </c>
       <c r="F66" s="105"/>
     </row>
-    <row r="67" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="67" spans="1:7" ht="15" outlineLevel="1">
       <c r="A67" s="153"/>
       <c r="B67" s="100"/>
       <c r="C67" s="101"/>
@@ -3431,7 +3450,7 @@
       </c>
       <c r="F67" s="105"/>
     </row>
-    <row r="68" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="68" spans="1:7" ht="15" outlineLevel="1">
       <c r="A68" s="153"/>
       <c r="B68" s="100"/>
       <c r="C68" s="101"/>
@@ -3442,7 +3461,7 @@
       </c>
       <c r="F68" s="105"/>
     </row>
-    <row r="69" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="69" spans="1:7" ht="15" outlineLevel="1">
       <c r="A69" s="153"/>
       <c r="B69" s="100"/>
       <c r="C69" s="101"/>
@@ -3453,7 +3472,7 @@
       </c>
       <c r="F69" s="105"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="70" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A70" s="153"/>
       <c r="B70" s="98" t="s">
         <v>186</v>
@@ -3466,7 +3485,7 @@
       </c>
       <c r="F70" s="104"/>
     </row>
-    <row r="71" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+    <row r="71" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A71" s="117">
         <v>3</v>
       </c>
@@ -3479,7 +3498,7 @@
       </c>
       <c r="D71" s="103">
         <f>D70-D57</f>
-        <v>0</v>
+        <v>-9746</v>
       </c>
       <c r="E71" s="126">
         <f>E70-E57</f>
@@ -4510,6 +4529,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4518,11 +4542,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4554,13 +4573,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4590,18 +4609,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4753,9 +4772,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4906,9 +4925,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5059,9 +5078,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="161"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5212,9 +5231,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="161"/>
-      <c r="D72" s="162"/>
-      <c r="E72" s="162"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5365,9 +5384,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="161"/>
-      <c r="D89" s="162"/>
-      <c r="E89" s="162"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5518,9 +5537,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="161"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5671,9 +5690,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="162"/>
-      <c r="E123" s="162"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5824,9 +5843,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="161"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="162"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5977,9 +5996,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="162"/>
-      <c r="E157" s="162"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6130,9 +6149,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="162"/>
-      <c r="E174" s="162"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6283,9 +6302,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="162"/>
-      <c r="E191" s="162"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6436,9 +6455,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="162"/>
-      <c r="E208" s="162"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6589,9 +6608,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="162"/>
-      <c r="E225" s="162"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6742,9 +6761,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="161"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6895,9 +6914,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="161"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7048,18 +7067,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="177"/>
-      <c r="D276" s="178"/>
-      <c r="E276" s="178"/>
+      <c r="C276" s="168"/>
+      <c r="D276" s="169"/>
+      <c r="E276" s="169"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="161"/>
-      <c r="D277" s="162"/>
-      <c r="E277" s="162"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7210,9 +7229,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="163"/>
-      <c r="D294" s="164"/>
-      <c r="E294" s="164"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7363,9 +7382,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="161"/>
-      <c r="D311" s="162"/>
-      <c r="E311" s="162"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7516,9 +7535,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="161"/>
-      <c r="D328" s="162"/>
-      <c r="E328" s="162"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7669,9 +7688,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="161"/>
-      <c r="D345" s="162"/>
-      <c r="E345" s="162"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7822,9 +7841,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="161"/>
-      <c r="D362" s="162"/>
-      <c r="E362" s="162"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7975,9 +7994,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="161"/>
-      <c r="D379" s="162"/>
-      <c r="E379" s="162"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8128,9 +8147,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="161"/>
-      <c r="D396" s="162"/>
-      <c r="E396" s="162"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8281,9 +8300,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="161"/>
-      <c r="D413" s="162"/>
-      <c r="E413" s="162"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8434,9 +8453,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="161"/>
-      <c r="D430" s="162"/>
-      <c r="E430" s="162"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8587,9 +8606,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="161"/>
-      <c r="D447" s="162"/>
-      <c r="E447" s="162"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8740,9 +8759,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="161"/>
-      <c r="D464" s="162"/>
-      <c r="E464" s="162"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8893,9 +8912,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="161"/>
-      <c r="D481" s="162"/>
-      <c r="E481" s="162"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9046,9 +9065,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="161"/>
-      <c r="D498" s="162"/>
-      <c r="E498" s="162"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9199,9 +9218,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="161"/>
-      <c r="D515" s="162"/>
-      <c r="E515" s="162"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9352,9 +9371,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="161"/>
-      <c r="D532" s="162"/>
-      <c r="E532" s="162"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9505,18 +9524,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="170"/>
+      <c r="D549" s="171"/>
+      <c r="E549" s="171"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="161"/>
-      <c r="D550" s="162"/>
-      <c r="E550" s="162"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9667,9 +9686,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="163"/>
-      <c r="D567" s="164"/>
-      <c r="E567" s="164"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9820,9 +9839,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="161"/>
-      <c r="D584" s="162"/>
-      <c r="E584" s="162"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9973,9 +9992,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="161"/>
-      <c r="D601" s="162"/>
-      <c r="E601" s="162"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10126,9 +10145,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="161"/>
-      <c r="D618" s="162"/>
-      <c r="E618" s="162"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10279,9 +10298,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="161"/>
-      <c r="D635" s="162"/>
-      <c r="E635" s="162"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10432,9 +10451,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="161"/>
-      <c r="D652" s="162"/>
-      <c r="E652" s="162"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10585,9 +10604,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="161"/>
-      <c r="D669" s="162"/>
-      <c r="E669" s="162"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10738,9 +10757,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="161"/>
-      <c r="D686" s="162"/>
-      <c r="E686" s="162"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10891,9 +10910,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="161"/>
-      <c r="D703" s="162"/>
-      <c r="E703" s="162"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11044,9 +11063,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="161"/>
-      <c r="D720" s="162"/>
-      <c r="E720" s="162"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11197,9 +11216,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="161"/>
-      <c r="D737" s="162"/>
-      <c r="E737" s="162"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11350,9 +11369,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="161"/>
-      <c r="D754" s="162"/>
-      <c r="E754" s="162"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11503,9 +11522,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="161"/>
-      <c r="D771" s="162"/>
-      <c r="E771" s="162"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11656,9 +11675,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="161"/>
-      <c r="D788" s="162"/>
-      <c r="E788" s="162"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11809,9 +11828,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="161"/>
-      <c r="D805" s="162"/>
-      <c r="E805" s="162"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11962,18 +11981,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="173"/>
-      <c r="D822" s="174"/>
-      <c r="E822" s="174"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="161"/>
-      <c r="D823" s="162"/>
-      <c r="E823" s="162"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12124,9 +12143,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="163"/>
-      <c r="D840" s="164"/>
-      <c r="E840" s="164"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12277,9 +12296,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="161"/>
-      <c r="D857" s="162"/>
-      <c r="E857" s="162"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12430,9 +12449,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="161"/>
-      <c r="D874" s="162"/>
-      <c r="E874" s="162"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12583,9 +12602,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="161"/>
-      <c r="D891" s="162"/>
-      <c r="E891" s="162"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12736,9 +12755,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="161"/>
-      <c r="D908" s="162"/>
-      <c r="E908" s="162"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12889,9 +12908,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="161"/>
-      <c r="D925" s="162"/>
-      <c r="E925" s="162"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13042,9 +13061,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="161"/>
-      <c r="D942" s="162"/>
-      <c r="E942" s="162"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13195,9 +13214,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="161"/>
-      <c r="D959" s="162"/>
-      <c r="E959" s="162"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13348,9 +13367,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="161"/>
-      <c r="D976" s="162"/>
-      <c r="E976" s="162"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13501,9 +13520,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="161"/>
-      <c r="D993" s="162"/>
-      <c r="E993" s="162"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13654,9 +13673,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="161"/>
-      <c r="D1010" s="162"/>
-      <c r="E1010" s="162"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13807,9 +13826,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="161"/>
-      <c r="D1027" s="162"/>
-      <c r="E1027" s="162"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13960,9 +13979,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="161"/>
-      <c r="D1044" s="162"/>
-      <c r="E1044" s="162"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14113,9 +14132,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="161"/>
-      <c r="D1061" s="162"/>
-      <c r="E1061" s="162"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14266,9 +14285,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="161"/>
-      <c r="D1078" s="162"/>
-      <c r="E1078" s="162"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14419,18 +14438,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="171"/>
-      <c r="D1095" s="172"/>
-      <c r="E1095" s="172"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="161"/>
-      <c r="D1096" s="162"/>
-      <c r="E1096" s="162"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14581,9 +14600,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="163"/>
-      <c r="D1113" s="164"/>
-      <c r="E1113" s="164"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14734,9 +14753,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="161"/>
-      <c r="D1130" s="162"/>
-      <c r="E1130" s="162"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14887,9 +14906,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="161"/>
-      <c r="D1147" s="162"/>
-      <c r="E1147" s="162"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15040,9 +15059,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="161"/>
-      <c r="D1164" s="162"/>
-      <c r="E1164" s="162"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15193,9 +15212,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="161"/>
-      <c r="D1181" s="162"/>
-      <c r="E1181" s="162"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15346,9 +15365,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="161"/>
-      <c r="D1198" s="162"/>
-      <c r="E1198" s="162"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15499,9 +15518,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="161"/>
-      <c r="D1215" s="162"/>
-      <c r="E1215" s="162"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15652,9 +15671,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="161"/>
-      <c r="D1232" s="162"/>
-      <c r="E1232" s="162"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15805,9 +15824,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="161"/>
-      <c r="D1249" s="162"/>
-      <c r="E1249" s="162"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15958,9 +15977,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="161"/>
-      <c r="D1266" s="162"/>
-      <c r="E1266" s="162"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16111,9 +16130,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="161"/>
-      <c r="D1283" s="162"/>
-      <c r="E1283" s="162"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16264,9 +16283,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="161"/>
-      <c r="D1300" s="162"/>
-      <c r="E1300" s="162"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16417,9 +16436,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="161"/>
-      <c r="D1317" s="162"/>
-      <c r="E1317" s="162"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16570,9 +16589,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="161"/>
-      <c r="D1334" s="162"/>
-      <c r="E1334" s="162"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16723,9 +16742,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="161"/>
-      <c r="D1351" s="162"/>
-      <c r="E1351" s="162"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16876,18 +16895,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="169"/>
-      <c r="D1368" s="170"/>
-      <c r="E1368" s="170"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="161"/>
-      <c r="D1369" s="162"/>
-      <c r="E1369" s="162"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17038,9 +17057,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="163"/>
-      <c r="D1386" s="164"/>
-      <c r="E1386" s="164"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17191,9 +17210,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="161"/>
-      <c r="D1403" s="162"/>
-      <c r="E1403" s="162"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17344,9 +17363,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="161"/>
-      <c r="D1420" s="162"/>
-      <c r="E1420" s="162"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17497,9 +17516,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="161"/>
-      <c r="D1437" s="162"/>
-      <c r="E1437" s="162"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17650,9 +17669,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="161"/>
-      <c r="D1454" s="162"/>
-      <c r="E1454" s="162"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17803,9 +17822,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="161"/>
-      <c r="D1471" s="162"/>
-      <c r="E1471" s="162"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17956,9 +17975,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="161"/>
-      <c r="D1488" s="162"/>
-      <c r="E1488" s="162"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18109,9 +18128,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="161"/>
-      <c r="D1505" s="162"/>
-      <c r="E1505" s="162"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18262,9 +18281,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="161"/>
-      <c r="D1522" s="162"/>
-      <c r="E1522" s="162"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18415,9 +18434,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="161"/>
-      <c r="D1539" s="162"/>
-      <c r="E1539" s="162"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18568,9 +18587,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="161"/>
-      <c r="D1556" s="162"/>
-      <c r="E1556" s="162"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18721,9 +18740,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="161"/>
-      <c r="D1573" s="162"/>
-      <c r="E1573" s="162"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18874,9 +18893,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="161"/>
-      <c r="D1590" s="162"/>
-      <c r="E1590" s="162"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19027,9 +19046,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="161"/>
-      <c r="D1607" s="162"/>
-      <c r="E1607" s="162"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19180,9 +19199,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="161"/>
-      <c r="D1624" s="162"/>
-      <c r="E1624" s="162"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19333,18 +19352,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="167"/>
-      <c r="D1641" s="168"/>
-      <c r="E1641" s="168"/>
+      <c r="C1641" s="178"/>
+      <c r="D1641" s="179"/>
+      <c r="E1641" s="179"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="161"/>
-      <c r="D1642" s="162"/>
-      <c r="E1642" s="162"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19495,9 +19514,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="163"/>
-      <c r="D1659" s="164"/>
-      <c r="E1659" s="164"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19648,9 +19667,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="161"/>
-      <c r="D1676" s="162"/>
-      <c r="E1676" s="162"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19801,9 +19820,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="161"/>
-      <c r="D1693" s="162"/>
-      <c r="E1693" s="162"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19954,9 +19973,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="161"/>
-      <c r="D1710" s="162"/>
-      <c r="E1710" s="162"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20107,9 +20126,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="161"/>
-      <c r="D1727" s="162"/>
-      <c r="E1727" s="162"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20260,9 +20279,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="161"/>
-      <c r="D1744" s="162"/>
-      <c r="E1744" s="162"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20413,9 +20432,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="161"/>
-      <c r="D1761" s="162"/>
-      <c r="E1761" s="162"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20566,9 +20585,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="161"/>
-      <c r="D1778" s="162"/>
-      <c r="E1778" s="162"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20719,9 +20738,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="161"/>
-      <c r="D1795" s="162"/>
-      <c r="E1795" s="162"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20872,9 +20891,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="161"/>
-      <c r="D1812" s="162"/>
-      <c r="E1812" s="162"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21025,9 +21044,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="161"/>
-      <c r="D1829" s="162"/>
-      <c r="E1829" s="162"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21178,9 +21197,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="161"/>
-      <c r="D1846" s="162"/>
-      <c r="E1846" s="162"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21331,9 +21350,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="161"/>
-      <c r="D1863" s="162"/>
-      <c r="E1863" s="162"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21484,9 +21503,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="161"/>
-      <c r="D1880" s="162"/>
-      <c r="E1880" s="162"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21637,9 +21656,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="161"/>
-      <c r="D1897" s="162"/>
-      <c r="E1897" s="162"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21790,18 +21809,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="165"/>
-      <c r="D1914" s="166"/>
-      <c r="E1914" s="166"/>
+      <c r="C1914" s="180"/>
+      <c r="D1914" s="181"/>
+      <c r="E1914" s="181"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="161"/>
-      <c r="D1915" s="162"/>
-      <c r="E1915" s="162"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21952,9 +21971,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="163"/>
-      <c r="D1932" s="164"/>
-      <c r="E1932" s="164"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22105,9 +22124,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="161"/>
-      <c r="D1949" s="162"/>
-      <c r="E1949" s="162"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22258,9 +22277,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="161"/>
-      <c r="D1966" s="162"/>
-      <c r="E1966" s="162"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22411,9 +22430,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="161"/>
-      <c r="D1983" s="162"/>
-      <c r="E1983" s="162"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22564,9 +22583,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="161"/>
-      <c r="D2000" s="162"/>
-      <c r="E2000" s="162"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22717,9 +22736,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="161"/>
-      <c r="D2017" s="162"/>
-      <c r="E2017" s="162"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22870,9 +22889,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="161"/>
-      <c r="D2034" s="162"/>
-      <c r="E2034" s="162"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23023,9 +23042,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="161"/>
-      <c r="D2051" s="162"/>
-      <c r="E2051" s="162"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23176,9 +23195,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="161"/>
-      <c r="D2068" s="162"/>
-      <c r="E2068" s="162"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23329,9 +23348,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="161"/>
-      <c r="D2085" s="162"/>
-      <c r="E2085" s="162"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23482,9 +23501,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="161"/>
-      <c r="D2102" s="162"/>
-      <c r="E2102" s="162"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23635,9 +23654,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="161"/>
-      <c r="D2119" s="162"/>
-      <c r="E2119" s="162"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23788,9 +23807,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="161"/>
-      <c r="D2136" s="162"/>
-      <c r="E2136" s="162"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23941,9 +23960,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="161"/>
-      <c r="D2153" s="162"/>
-      <c r="E2153" s="162"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24094,9 +24113,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="161"/>
-      <c r="D2170" s="162"/>
-      <c r="E2170" s="162"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24244,26 +24263,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24276,113 +24380,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25133,7 +25152,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25344,7 +25363,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25617,7 +25636,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25639,163 +25658,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="207"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="215" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="204"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="210"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="208" t="s">
+      <c r="A5" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="209"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="214" t="s">
+      <c r="A7" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="215"/>
+      <c r="B7" s="202"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="203" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="213"/>
+      <c r="B9" s="204"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="206"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="197" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="214" t="s">
+      <c r="A19" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="215"/>
+      <c r="B19" s="202"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="203" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="213"/>
+      <c r="B21" s="204"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="199"/>
-      <c r="B22" s="200"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="206"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25806,6 +25812,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>